<commit_message>
updated zeitplan: added phase 0 and updated tasks
</commit_message>
<xml_diff>
--- a/docs/Zeitplan.xlsx
+++ b/docs/Zeitplan.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:11_{73B3F47B-72C8-4FAC-A7F2-7AE807A63BB5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E5E4A6B-CB20-426E-BCD2-ADC8028DA0CB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="11949" tabRatio="415" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
   <si>
     <t>Erstellen Sie auf diesem Arbeitsblatt ein Gantt-Diagramm.
 Geben Sie den Titel dieses Projekts in Zelle B1 ein. 
@@ -84,21 +84,6 @@
   </si>
   <si>
     <t>Meilensteinbeschreibung</t>
-  </si>
-  <si>
-    <t>Aufgabe 1</t>
-  </si>
-  <si>
-    <t>Aufgabe 2</t>
-  </si>
-  <si>
-    <t>Aufgabe 3</t>
-  </si>
-  <si>
-    <t>Aufgabe 4</t>
-  </si>
-  <si>
-    <t>Aufgabe 5</t>
   </si>
   <si>
     <t>Um weitere Daten hinzuzufügen, fügen Sie neue Zeilen ÜBER dieser ein.</t>
@@ -173,25 +158,52 @@
     <t>Genereller Aufbaumöglichkeiten definieren</t>
   </si>
   <si>
-    <t>Raspberry Pi mit obl. Sensoren und Aktuatoren ausprobieren</t>
-  </si>
-  <si>
-    <t>Logging Interface designen</t>
-  </si>
-  <si>
-    <t>Logging Interface implementieren</t>
-  </si>
-  <si>
-    <t>MVP finalisieren</t>
-  </si>
-  <si>
     <t>MVP dokumentieren</t>
   </si>
   <si>
-    <t>Grove Anschlüsse ausprobieren</t>
+    <t>Phase 0: Vorbereitung</t>
   </si>
   <si>
-    <t>Projekt finalisieren</t>
+    <t>Grove Anschlüsse kennenlernen und Beispiele implementieren</t>
+  </si>
+  <si>
+    <t>Raspberry Pi mit obl. Sensoren und Aktuatoren kennenlernen und Beispiele implementieren</t>
+  </si>
+  <si>
+    <t>Grove Anschluss fertigstellen</t>
+  </si>
+  <si>
+    <t>MVP fertigstellen</t>
+  </si>
+  <si>
+    <t>Projekt fertigstellen</t>
+  </si>
+  <si>
+    <t>Integration der Grove Anschlüsse im GPIO-Simulator: Architektur und Dokumentation</t>
+  </si>
+  <si>
+    <t>Logging Interface: Architektur und Dokumentation</t>
+  </si>
+  <si>
+    <t>Integration der Grove Anschlüsse im GPIO-Simulator: Implementation</t>
+  </si>
+  <si>
+    <t>Logging Interface: Implementieren</t>
+  </si>
+  <si>
+    <t>Mockup für User Interface erstellen</t>
+  </si>
+  <si>
+    <t>Simulator UI: Front End</t>
+  </si>
+  <si>
+    <t>Simulator UI: Back End</t>
+  </si>
+  <si>
+    <t>User Guide schreiben</t>
+  </si>
+  <si>
+    <t>Beispiel-Projekt implementieren</t>
   </si>
 </sst>
 </file>
@@ -1121,6 +1133,21 @@
     <xf numFmtId="14" fontId="16" fillId="0" borderId="0" xfId="9" applyFill="1" applyBorder="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="25" fillId="37" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="37" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="25" fillId="37" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="25" fillId="37" borderId="0" xfId="9" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="25" fillId="37" borderId="0" xfId="10" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="8" applyFont="1">
       <alignment horizontal="right" vertical="center" indent="1"/>
     </xf>
@@ -1138,21 +1165,6 @@
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="2" xfId="8" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="37" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="37" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="25" fillId="37" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="25" fillId="37" borderId="0" xfId="9" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="168" fontId="25" fillId="37" borderId="0" xfId="10" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="50">
@@ -1498,7 +1510,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp1.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Scroll" dx="39" fmlaLink="$E$3" horiz="1" max="365" page="0" val="47"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Scroll" dx="39" fmlaLink="$E$3" horiz="1" max="365" page="0" val="53"/>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1514,7 +1526,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>12</xdr:col>
-          <xdr:colOff>47624</xdr:colOff>
+          <xdr:colOff>48986</xdr:colOff>
           <xdr:row>2</xdr:row>
           <xdr:rowOff>342900</xdr:rowOff>
         </xdr:to>
@@ -1557,8 +1569,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Meilensteine" displayName="Meilensteine" ref="B6:F30" totalsRowShown="0">
-  <autoFilter ref="B6:F30" xr:uid="{00000000-0009-0000-0100-000001000000}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Meilensteine" displayName="Meilensteine" ref="B6:F31" totalsRowShown="0">
+  <autoFilter ref="B6:F31" xr:uid="{00000000-0009-0000-0100-000001000000}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -1844,10 +1856,10 @@
   <sheetPr codeName="Sheet1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:BK33"/>
+  <dimension ref="A1:BK34"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="B6" zoomScale="69" zoomScaleNormal="50" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="V19" sqref="V19"/>
+    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="A3" zoomScale="69" zoomScaleNormal="50" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.06640625" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.45"/>
@@ -1867,7 +1879,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="15" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="C1" s="1"/>
       <c r="E1"/>
@@ -1877,18 +1889,18 @@
     </row>
     <row r="2" spans="1:63" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A2" s="13" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="B2" s="16"/>
-      <c r="C2" s="53" t="s">
-        <v>16</v>
-      </c>
-      <c r="D2" s="54"/>
-      <c r="E2" s="55">
+      <c r="C2" s="58" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="59"/>
+      <c r="E2" s="60">
         <f ca="1">IFERROR(IF(MIN(Meilensteine[Start])=0,TODAY(),MIN(Meilensteine[Start])),TODAY())</f>
         <v>43864</v>
       </c>
-      <c r="F2" s="56"/>
+      <c r="F2" s="61"/>
       <c r="I2" s="36"/>
       <c r="J2" s="36"/>
       <c r="K2" s="36"/>
@@ -1901,12 +1913,12 @@
         <v>1</v>
       </c>
       <c r="B3" s="16"/>
-      <c r="C3" s="53" t="s">
-        <v>17</v>
-      </c>
-      <c r="D3" s="54"/>
+      <c r="C3" s="58" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="59"/>
       <c r="E3" s="39">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="H3" s="46"/>
       <c r="I3" s="47"/>
@@ -1919,10 +1931,10 @@
       <c r="A4" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="57" t="s">
-        <v>18</v>
-      </c>
-      <c r="D4" s="58"/>
+      <c r="C4" s="62" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="63"/>
       <c r="E4" s="40">
         <v>1</v>
       </c>
@@ -1942,7 +1954,7 @@
       <c r="N4" s="17"/>
       <c r="O4" s="17" t="str">
         <f ca="1">IF(TEXT(O5,"MMMM")=H4,"",TEXT(O5,"MMMM"))</f>
-        <v/>
+        <v>April</v>
       </c>
       <c r="P4" s="17"/>
       <c r="Q4" s="17"/>
@@ -1952,7 +1964,7 @@
       <c r="U4" s="17"/>
       <c r="V4" s="17" t="str">
         <f ca="1">IF(OR(TEXT(V5,"MMMM")=O4,TEXT(V5,"MMMM")=H4),"",TEXT(V5,"MMMM"))</f>
-        <v>April</v>
+        <v/>
       </c>
       <c r="W4" s="17"/>
       <c r="X4" s="17"/>
@@ -1982,7 +1994,7 @@
       <c r="AP4" s="17"/>
       <c r="AQ4" s="17" t="str">
         <f ca="1">IF(OR(TEXT(AQ5,"MMMM")=AJ4,TEXT(AQ5,"MMMM")=AC4,TEXT(AQ5,"MMMM")=V4,TEXT(AQ5,"MMMM")=O4),"",TEXT(AQ5,"MMMM"))</f>
-        <v/>
+        <v>Mai</v>
       </c>
       <c r="AR4" s="17"/>
       <c r="AS4" s="17"/>
@@ -1992,7 +2004,7 @@
       <c r="AW4" s="17"/>
       <c r="AX4" s="17" t="str">
         <f ca="1">IF(OR(TEXT(AX5,"MMMM")=AQ4,TEXT(AX5,"MMMM")=AJ4,TEXT(AX5,"MMMM")=AC4,TEXT(AX5,"MMMM")=V4),"",TEXT(AX5,"MMMM"))</f>
-        <v>Mai</v>
+        <v/>
       </c>
       <c r="AY4" s="17"/>
       <c r="AZ4" s="17"/>
@@ -2019,227 +2031,227 @@
       <c r="G5" s="35"/>
       <c r="H5" s="48">
         <f ca="1">IFERROR(Projekt_Start+Scroll_Schrittweite,TODAY())</f>
-        <v>43911</v>
+        <v>43917</v>
       </c>
       <c r="I5" s="49">
         <f ca="1">H5+1</f>
-        <v>43912</v>
+        <v>43918</v>
       </c>
       <c r="J5" s="50">
         <f t="shared" ref="J5:AW5" ca="1" si="0">I5+1</f>
-        <v>43913</v>
+        <v>43919</v>
       </c>
       <c r="K5" s="50">
         <f ca="1">J5+1</f>
-        <v>43914</v>
+        <v>43920</v>
       </c>
       <c r="L5" s="50">
         <f t="shared" ca="1" si="0"/>
-        <v>43915</v>
+        <v>43921</v>
       </c>
       <c r="M5" s="50">
         <f t="shared" ca="1" si="0"/>
-        <v>43916</v>
+        <v>43922</v>
       </c>
       <c r="N5" s="50">
         <f t="shared" ca="1" si="0"/>
-        <v>43917</v>
+        <v>43923</v>
       </c>
       <c r="O5" s="50">
         <f ca="1">N5+1</f>
-        <v>43918</v>
+        <v>43924</v>
       </c>
       <c r="P5" s="50">
         <f ca="1">O5+1</f>
-        <v>43919</v>
+        <v>43925</v>
       </c>
       <c r="Q5" s="50">
         <f t="shared" ca="1" si="0"/>
-        <v>43920</v>
+        <v>43926</v>
       </c>
       <c r="R5" s="50">
         <f t="shared" ca="1" si="0"/>
-        <v>43921</v>
+        <v>43927</v>
       </c>
       <c r="S5" s="50">
         <f t="shared" ca="1" si="0"/>
-        <v>43922</v>
+        <v>43928</v>
       </c>
       <c r="T5" s="50">
         <f t="shared" ca="1" si="0"/>
-        <v>43923</v>
+        <v>43929</v>
       </c>
       <c r="U5" s="50">
         <f t="shared" ca="1" si="0"/>
-        <v>43924</v>
+        <v>43930</v>
       </c>
       <c r="V5" s="50">
         <f ca="1">U5+1</f>
-        <v>43925</v>
+        <v>43931</v>
       </c>
       <c r="W5" s="50">
         <f ca="1">V5+1</f>
-        <v>43926</v>
+        <v>43932</v>
       </c>
       <c r="X5" s="50">
         <f t="shared" ca="1" si="0"/>
-        <v>43927</v>
+        <v>43933</v>
       </c>
       <c r="Y5" s="50">
         <f t="shared" ca="1" si="0"/>
-        <v>43928</v>
+        <v>43934</v>
       </c>
       <c r="Z5" s="50">
         <f t="shared" ca="1" si="0"/>
-        <v>43929</v>
+        <v>43935</v>
       </c>
       <c r="AA5" s="50">
         <f t="shared" ca="1" si="0"/>
-        <v>43930</v>
+        <v>43936</v>
       </c>
       <c r="AB5" s="50">
         <f t="shared" ca="1" si="0"/>
-        <v>43931</v>
+        <v>43937</v>
       </c>
       <c r="AC5" s="50">
         <f ca="1">AB5+1</f>
-        <v>43932</v>
+        <v>43938</v>
       </c>
       <c r="AD5" s="50">
         <f ca="1">AC5+1</f>
-        <v>43933</v>
+        <v>43939</v>
       </c>
       <c r="AE5" s="50">
         <f t="shared" ca="1" si="0"/>
-        <v>43934</v>
+        <v>43940</v>
       </c>
       <c r="AF5" s="50">
         <f t="shared" ca="1" si="0"/>
-        <v>43935</v>
+        <v>43941</v>
       </c>
       <c r="AG5" s="50">
         <f t="shared" ca="1" si="0"/>
-        <v>43936</v>
+        <v>43942</v>
       </c>
       <c r="AH5" s="50">
         <f t="shared" ca="1" si="0"/>
-        <v>43937</v>
+        <v>43943</v>
       </c>
       <c r="AI5" s="50">
         <f t="shared" ca="1" si="0"/>
-        <v>43938</v>
+        <v>43944</v>
       </c>
       <c r="AJ5" s="50">
         <f ca="1">AI5+1</f>
-        <v>43939</v>
+        <v>43945</v>
       </c>
       <c r="AK5" s="50">
         <f ca="1">AJ5+1</f>
-        <v>43940</v>
+        <v>43946</v>
       </c>
       <c r="AL5" s="50">
         <f t="shared" ca="1" si="0"/>
-        <v>43941</v>
+        <v>43947</v>
       </c>
       <c r="AM5" s="50">
         <f t="shared" ca="1" si="0"/>
-        <v>43942</v>
+        <v>43948</v>
       </c>
       <c r="AN5" s="50">
         <f t="shared" ca="1" si="0"/>
-        <v>43943</v>
+        <v>43949</v>
       </c>
       <c r="AO5" s="50">
         <f t="shared" ca="1" si="0"/>
-        <v>43944</v>
+        <v>43950</v>
       </c>
       <c r="AP5" s="50">
         <f t="shared" ca="1" si="0"/>
-        <v>43945</v>
+        <v>43951</v>
       </c>
       <c r="AQ5" s="50">
         <f ca="1">AP5+1</f>
-        <v>43946</v>
+        <v>43952</v>
       </c>
       <c r="AR5" s="50">
         <f ca="1">AQ5+1</f>
-        <v>43947</v>
+        <v>43953</v>
       </c>
       <c r="AS5" s="50">
         <f t="shared" ca="1" si="0"/>
-        <v>43948</v>
+        <v>43954</v>
       </c>
       <c r="AT5" s="50">
         <f t="shared" ca="1" si="0"/>
-        <v>43949</v>
+        <v>43955</v>
       </c>
       <c r="AU5" s="50">
         <f t="shared" ca="1" si="0"/>
-        <v>43950</v>
+        <v>43956</v>
       </c>
       <c r="AV5" s="50">
         <f t="shared" ca="1" si="0"/>
-        <v>43951</v>
+        <v>43957</v>
       </c>
       <c r="AW5" s="50">
         <f t="shared" ca="1" si="0"/>
-        <v>43952</v>
+        <v>43958</v>
       </c>
       <c r="AX5" s="50">
         <f ca="1">AW5+1</f>
-        <v>43953</v>
+        <v>43959</v>
       </c>
       <c r="AY5" s="50">
         <f ca="1">AX5+1</f>
-        <v>43954</v>
+        <v>43960</v>
       </c>
       <c r="AZ5" s="50">
         <f t="shared" ref="AZ5:BD5" ca="1" si="1">AY5+1</f>
-        <v>43955</v>
+        <v>43961</v>
       </c>
       <c r="BA5" s="50">
         <f t="shared" ca="1" si="1"/>
-        <v>43956</v>
+        <v>43962</v>
       </c>
       <c r="BB5" s="50">
         <f t="shared" ca="1" si="1"/>
-        <v>43957</v>
+        <v>43963</v>
       </c>
       <c r="BC5" s="50">
         <f t="shared" ca="1" si="1"/>
-        <v>43958</v>
+        <v>43964</v>
       </c>
       <c r="BD5" s="50">
         <f t="shared" ca="1" si="1"/>
-        <v>43959</v>
+        <v>43965</v>
       </c>
       <c r="BE5" s="50">
         <f ca="1">BD5+1</f>
-        <v>43960</v>
+        <v>43966</v>
       </c>
       <c r="BF5" s="50">
         <f ca="1">BE5+1</f>
-        <v>43961</v>
+        <v>43967</v>
       </c>
       <c r="BG5" s="50">
         <f t="shared" ref="BG5:BK5" ca="1" si="2">BF5+1</f>
-        <v>43962</v>
+        <v>43968</v>
       </c>
       <c r="BH5" s="50">
         <f t="shared" ca="1" si="2"/>
-        <v>43963</v>
+        <v>43969</v>
       </c>
       <c r="BI5" s="50">
         <f t="shared" ca="1" si="2"/>
-        <v>43964</v>
+        <v>43970</v>
       </c>
       <c r="BJ5" s="50">
         <f t="shared" ca="1" si="2"/>
-        <v>43965</v>
+        <v>43971</v>
       </c>
       <c r="BK5" s="51">
         <f t="shared" ca="1" si="2"/>
-        <v>43966</v>
+        <v>43972</v>
       </c>
     </row>
     <row r="6" spans="1:63" ht="31" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
@@ -2250,21 +2262,21 @@
         <v>9</v>
       </c>
       <c r="C6" s="23" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="D6" s="23" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="E6" s="23" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="F6" s="23" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="G6" s="21"/>
       <c r="H6" s="42" t="str">
         <f t="shared" ref="H6:AM6" ca="1" si="3">LEFT(TEXT(H5,"TTT"),1)</f>
-        <v>S</v>
+        <v>F</v>
       </c>
       <c r="I6" s="43" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -2272,27 +2284,27 @@
       </c>
       <c r="J6" s="45" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>M</v>
+        <v>S</v>
       </c>
       <c r="K6" s="44" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>D</v>
+        <v>M</v>
       </c>
       <c r="L6" s="44" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>M</v>
+        <v>D</v>
       </c>
       <c r="M6" s="44" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>D</v>
+        <v>M</v>
       </c>
       <c r="N6" s="44" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>F</v>
+        <v>D</v>
       </c>
       <c r="O6" s="44" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>S</v>
+        <v>F</v>
       </c>
       <c r="P6" s="44" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -2300,27 +2312,27 @@
       </c>
       <c r="Q6" s="44" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>M</v>
+        <v>S</v>
       </c>
       <c r="R6" s="44" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>D</v>
+        <v>M</v>
       </c>
       <c r="S6" s="44" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>M</v>
+        <v>D</v>
       </c>
       <c r="T6" s="44" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>D</v>
+        <v>M</v>
       </c>
       <c r="U6" s="44" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>F</v>
+        <v>D</v>
       </c>
       <c r="V6" s="44" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>S</v>
+        <v>F</v>
       </c>
       <c r="W6" s="44" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -2328,27 +2340,27 @@
       </c>
       <c r="X6" s="44" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>M</v>
+        <v>S</v>
       </c>
       <c r="Y6" s="44" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>D</v>
+        <v>M</v>
       </c>
       <c r="Z6" s="44" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>M</v>
+        <v>D</v>
       </c>
       <c r="AA6" s="44" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>D</v>
+        <v>M</v>
       </c>
       <c r="AB6" s="44" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>F</v>
+        <v>D</v>
       </c>
       <c r="AC6" s="44" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>S</v>
+        <v>F</v>
       </c>
       <c r="AD6" s="44" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -2356,27 +2368,27 @@
       </c>
       <c r="AE6" s="44" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>M</v>
+        <v>S</v>
       </c>
       <c r="AF6" s="44" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>D</v>
+        <v>M</v>
       </c>
       <c r="AG6" s="44" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>M</v>
+        <v>D</v>
       </c>
       <c r="AH6" s="44" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>D</v>
+        <v>M</v>
       </c>
       <c r="AI6" s="44" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>F</v>
+        <v>D</v>
       </c>
       <c r="AJ6" s="44" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>S</v>
+        <v>F</v>
       </c>
       <c r="AK6" s="44" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -2384,27 +2396,27 @@
       </c>
       <c r="AL6" s="44" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>M</v>
+        <v>S</v>
       </c>
       <c r="AM6" s="44" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>D</v>
+        <v>M</v>
       </c>
       <c r="AN6" s="44" t="str">
         <f t="shared" ref="AN6:BK6" ca="1" si="4">LEFT(TEXT(AN5,"TTT"),1)</f>
-        <v>M</v>
+        <v>D</v>
       </c>
       <c r="AO6" s="44" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>D</v>
+        <v>M</v>
       </c>
       <c r="AP6" s="44" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>F</v>
+        <v>D</v>
       </c>
       <c r="AQ6" s="44" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>S</v>
+        <v>F</v>
       </c>
       <c r="AR6" s="44" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -2412,27 +2424,27 @@
       </c>
       <c r="AS6" s="44" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>M</v>
+        <v>S</v>
       </c>
       <c r="AT6" s="44" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>D</v>
+        <v>M</v>
       </c>
       <c r="AU6" s="44" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>M</v>
+        <v>D</v>
       </c>
       <c r="AV6" s="44" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>D</v>
+        <v>M</v>
       </c>
       <c r="AW6" s="44" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>F</v>
+        <v>D</v>
       </c>
       <c r="AX6" s="44" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>S</v>
+        <v>F</v>
       </c>
       <c r="AY6" s="44" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -2440,27 +2452,27 @@
       </c>
       <c r="AZ6" s="44" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>M</v>
+        <v>S</v>
       </c>
       <c r="BA6" s="44" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>D</v>
+        <v>M</v>
       </c>
       <c r="BB6" s="44" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>M</v>
+        <v>D</v>
       </c>
       <c r="BC6" s="44" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>D</v>
+        <v>M</v>
       </c>
       <c r="BD6" s="44" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>F</v>
+        <v>D</v>
       </c>
       <c r="BE6" s="44" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>S</v>
+        <v>F</v>
       </c>
       <c r="BF6" s="44" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -2468,23 +2480,23 @@
       </c>
       <c r="BG6" s="44" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>M</v>
+        <v>S</v>
       </c>
       <c r="BH6" s="44" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>D</v>
+        <v>M</v>
       </c>
       <c r="BI6" s="44" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>M</v>
+        <v>D</v>
       </c>
       <c r="BJ6" s="44" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>D</v>
+        <v>M</v>
       </c>
       <c r="BK6" s="44" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>F</v>
+        <v>D</v>
       </c>
     </row>
     <row r="7" spans="1:63" ht="30" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
@@ -2557,15 +2569,15 @@
       <c r="A8" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="59" t="s">
+      <c r="B8" s="53" t="s">
         <v>32</v>
       </c>
-      <c r="C8" s="60"/>
-      <c r="D8" s="61"/>
-      <c r="E8" s="62">
+      <c r="C8" s="54"/>
+      <c r="D8" s="55"/>
+      <c r="E8" s="56">
         <v>43864</v>
       </c>
-      <c r="F8" s="63"/>
+      <c r="F8" s="57"/>
       <c r="G8" s="20"/>
       <c r="H8" s="29" t="str">
         <f>IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(H$5=$E8,$F8=1),Meilenstein_Markierung,"")),"")</f>
@@ -2793,15 +2805,15 @@
       </c>
     </row>
     <row r="9" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A9" s="13"/>
+      <c r="A9" s="12"/>
       <c r="B9" s="31" t="s">
-        <v>29</v>
-      </c>
-      <c r="C9" s="27"/>
+        <v>24</v>
+      </c>
+      <c r="C9" s="23"/>
       <c r="D9" s="24">
         <v>1</v>
       </c>
-      <c r="E9" s="52">
+      <c r="E9" s="25">
         <v>43864</v>
       </c>
       <c r="F9" s="26">
@@ -3034,15 +3046,15 @@
       </c>
     </row>
     <row r="10" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A10" s="13"/>
+      <c r="A10" s="12"/>
       <c r="B10" s="31" t="s">
-        <v>30</v>
-      </c>
-      <c r="C10" s="27"/>
+        <v>25</v>
+      </c>
+      <c r="C10" s="23"/>
       <c r="D10" s="24">
         <v>1</v>
       </c>
-      <c r="E10" s="52">
+      <c r="E10" s="25">
         <v>43881</v>
       </c>
       <c r="F10" s="26">
@@ -3276,500 +3288,158 @@
     </row>
     <row r="11" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A11" s="12"/>
-      <c r="B11" s="31" t="s">
-        <v>31</v>
-      </c>
-      <c r="C11" s="27"/>
-      <c r="D11" s="24">
-        <v>1</v>
-      </c>
-      <c r="E11" s="52">
-        <v>43881</v>
-      </c>
-      <c r="F11" s="26">
-        <v>15</v>
-      </c>
+      <c r="B11" s="53" t="s">
+        <v>27</v>
+      </c>
+      <c r="C11" s="54"/>
+      <c r="D11" s="55"/>
+      <c r="E11" s="56"/>
+      <c r="F11" s="57"/>
       <c r="G11" s="20"/>
-      <c r="H11" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(H$5=$E11,$F11=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="I11" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(I$5=$E11,$F11=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="J11" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(J$5=$E11,$F11=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="K11" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(K$5=$E11,$F11=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="L11" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(L$5=$E11,$F11=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="M11" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(M$5=$E11,$F11=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="N11" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(N$5=$E11,$F11=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="O11" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(O$5=$E11,$F11=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="P11" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(P$5=$E11,$F11=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="Q11" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(Q$5=$E11,$F11=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="R11" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(R$5=$E11,$F11=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="S11" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(S$5=$E11,$F11=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="T11" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(T$5=$E11,$F11=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="U11" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(U$5=$E11,$F11=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="V11" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(V$5=$E11,$F11=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="W11" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(W$5=$E11,$F11=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="X11" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(X$5=$E11,$F11=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="Y11" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(Y$5=$E11,$F11=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="Z11" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(Z$5=$E11,$F11=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="AA11" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AA$5=$E11,$F11=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="AB11" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AB$5=$E11,$F11=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="AC11" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AC$5=$E11,$F11=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="AD11" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AD$5=$E11,$F11=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="AE11" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AE$5=$E11,$F11=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="AF11" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AF$5=$E11,$F11=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="AG11" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AG$5=$E11,$F11=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="AH11" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AH$5=$E11,$F11=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="AI11" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AI$5=$E11,$F11=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="AJ11" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AJ$5=$E11,$F11=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="AK11" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AK$5=$E11,$F11=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="AL11" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AL$5=$E11,$F11=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="AM11" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AM$5=$E11,$F11=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="AN11" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AN$5=$E11,$F11=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="AO11" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AO$5=$E11,$F11=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="AP11" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AP$5=$E11,$F11=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="AQ11" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AQ$5=$E11,$F11=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="AR11" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AR$5=$E11,$F11=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="AS11" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AS$5=$E11,$F11=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="AT11" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AT$5=$E11,$F11=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="AU11" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AU$5=$E11,$F11=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="AV11" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AV$5=$E11,$F11=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="AW11" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AW$5=$E11,$F11=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="AX11" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AX$5=$E11,$F11=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="AY11" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AY$5=$E11,$F11=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="AZ11" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AZ$5=$E11,$F11=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="BA11" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(BA$5=$E11,$F11=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="BB11" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(BB$5=$E11,$F11=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="BC11" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(BC$5=$E11,$F11=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="BD11" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(BD$5=$E11,$F11=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="BE11" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(BE$5=$E11,$F11=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="BF11" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(BF$5=$E11,$F11=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="BG11" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(BG$5=$E11,$F11=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="BH11" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(BH$5=$E11,$F11=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="BI11" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(BI$5=$E11,$F11=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="BJ11" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(BJ$5=$E11,$F11=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="BK11" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(BK$5=$E11,$F11=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
+      <c r="H11" s="29"/>
+      <c r="I11" s="29"/>
+      <c r="J11" s="29"/>
+      <c r="K11" s="29"/>
+      <c r="L11" s="29"/>
+      <c r="M11" s="29"/>
+      <c r="N11" s="29"/>
+      <c r="O11" s="29"/>
+      <c r="P11" s="29"/>
+      <c r="Q11" s="29"/>
+      <c r="R11" s="29"/>
+      <c r="S11" s="29"/>
+      <c r="T11" s="29"/>
+      <c r="U11" s="29"/>
+      <c r="V11" s="29"/>
+      <c r="W11" s="29"/>
+      <c r="X11" s="29"/>
+      <c r="Y11" s="29"/>
+      <c r="Z11" s="29"/>
+      <c r="AA11" s="29"/>
+      <c r="AB11" s="29"/>
+      <c r="AC11" s="29"/>
+      <c r="AD11" s="29"/>
+      <c r="AE11" s="29"/>
+      <c r="AF11" s="29"/>
+      <c r="AG11" s="29"/>
+      <c r="AH11" s="29"/>
+      <c r="AI11" s="29"/>
+      <c r="AJ11" s="29"/>
+      <c r="AK11" s="29"/>
+      <c r="AL11" s="29"/>
+      <c r="AM11" s="29"/>
+      <c r="AN11" s="29"/>
+      <c r="AO11" s="29"/>
+      <c r="AP11" s="29"/>
+      <c r="AQ11" s="29"/>
+      <c r="AR11" s="29"/>
+      <c r="AS11" s="29"/>
+      <c r="AT11" s="29"/>
+      <c r="AU11" s="29"/>
+      <c r="AV11" s="29"/>
+      <c r="AW11" s="29"/>
+      <c r="AX11" s="29"/>
+      <c r="AY11" s="29"/>
+      <c r="AZ11" s="29"/>
+      <c r="BA11" s="29"/>
+      <c r="BB11" s="29"/>
+      <c r="BC11" s="29"/>
+      <c r="BD11" s="29"/>
+      <c r="BE11" s="29"/>
+      <c r="BF11" s="29"/>
+      <c r="BG11" s="29"/>
+      <c r="BH11" s="29"/>
+      <c r="BI11" s="29"/>
+      <c r="BJ11" s="29"/>
+      <c r="BK11" s="29"/>
     </row>
     <row r="12" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A12" s="12"/>
       <c r="B12" s="31" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="C12" s="27"/>
       <c r="D12" s="24">
         <v>1</v>
       </c>
       <c r="E12" s="52">
-        <v>43895</v>
+        <v>43881</v>
       </c>
       <c r="F12" s="26">
         <v>15</v>
       </c>
       <c r="G12" s="20"/>
-      <c r="H12" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(H$5=$E12,$F12=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="I12" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(I$5=$E12,$F12=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="J12" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(J$5=$E12,$F12=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="K12" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(K$5=$E12,$F12=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="L12" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(L$5=$E12,$F12=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="M12" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(M$5=$E12,$F12=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="N12" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(N$5=$E12,$F12=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="O12" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(O$5=$E12,$F12=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="P12" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(P$5=$E12,$F12=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="Q12" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(Q$5=$E12,$F12=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="R12" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(R$5=$E12,$F12=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="S12" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(S$5=$E12,$F12=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="T12" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(T$5=$E12,$F12=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="U12" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(U$5=$E12,$F12=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="V12" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(V$5=$E12,$F12=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="W12" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(W$5=$E12,$F12=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="X12" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(X$5=$E12,$F12=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="Y12" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(Y$5=$E12,$F12=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="Z12" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(Z$5=$E12,$F12=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="AA12" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AA$5=$E12,$F12=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="AB12" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AB$5=$E12,$F12=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="AC12" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AC$5=$E12,$F12=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="AD12" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AD$5=$E12,$F12=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="AE12" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AE$5=$E12,$F12=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="AF12" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AF$5=$E12,$F12=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="AG12" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AG$5=$E12,$F12=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="AH12" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AH$5=$E12,$F12=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="AI12" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AI$5=$E12,$F12=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="AJ12" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AJ$5=$E12,$F12=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="AK12" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AK$5=$E12,$F12=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="AL12" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AL$5=$E12,$F12=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="AM12" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AM$5=$E12,$F12=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="AN12" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AN$5=$E12,$F12=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="AO12" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AO$5=$E12,$F12=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="AP12" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AP$5=$E12,$F12=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="AQ12" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AQ$5=$E12,$F12=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="AR12" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AR$5=$E12,$F12=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="AS12" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AS$5=$E12,$F12=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="AT12" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AT$5=$E12,$F12=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="AU12" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AU$5=$E12,$F12=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="AV12" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AV$5=$E12,$F12=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="AW12" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AW$5=$E12,$F12=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="AX12" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AX$5=$E12,$F12=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="AY12" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AY$5=$E12,$F12=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="AZ12" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AZ$5=$E12,$F12=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="BA12" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(BA$5=$E12,$F12=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="BB12" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(BB$5=$E12,$F12=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="BC12" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(BC$5=$E12,$F12=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="BD12" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(BD$5=$E12,$F12=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="BE12" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(BE$5=$E12,$F12=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="BF12" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(BF$5=$E12,$F12=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="BG12" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(BG$5=$E12,$F12=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="BH12" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(BH$5=$E12,$F12=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="BI12" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(BI$5=$E12,$F12=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="BJ12" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(BJ$5=$E12,$F12=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="BK12" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(BK$5=$E12,$F12=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
+      <c r="H12" s="29"/>
+      <c r="I12" s="29"/>
+      <c r="J12" s="29"/>
+      <c r="K12" s="29"/>
+      <c r="L12" s="29"/>
+      <c r="M12" s="29"/>
+      <c r="N12" s="29"/>
+      <c r="O12" s="29"/>
+      <c r="P12" s="29"/>
+      <c r="Q12" s="29"/>
+      <c r="R12" s="29"/>
+      <c r="S12" s="29"/>
+      <c r="T12" s="29"/>
+      <c r="U12" s="29"/>
+      <c r="V12" s="29"/>
+      <c r="W12" s="29"/>
+      <c r="X12" s="29"/>
+      <c r="Y12" s="29"/>
+      <c r="Z12" s="29"/>
+      <c r="AA12" s="29"/>
+      <c r="AB12" s="29"/>
+      <c r="AC12" s="29"/>
+      <c r="AD12" s="29"/>
+      <c r="AE12" s="29"/>
+      <c r="AF12" s="29"/>
+      <c r="AG12" s="29"/>
+      <c r="AH12" s="29"/>
+      <c r="AI12" s="29"/>
+      <c r="AJ12" s="29"/>
+      <c r="AK12" s="29"/>
+      <c r="AL12" s="29"/>
+      <c r="AM12" s="29"/>
+      <c r="AN12" s="29"/>
+      <c r="AO12" s="29"/>
+      <c r="AP12" s="29"/>
+      <c r="AQ12" s="29"/>
+      <c r="AR12" s="29"/>
+      <c r="AS12" s="29"/>
+      <c r="AT12" s="29"/>
+      <c r="AU12" s="29"/>
+      <c r="AV12" s="29"/>
+      <c r="AW12" s="29"/>
+      <c r="AX12" s="29"/>
+      <c r="AY12" s="29"/>
+      <c r="AZ12" s="29"/>
+      <c r="BA12" s="29"/>
+      <c r="BB12" s="29"/>
+      <c r="BC12" s="29"/>
+      <c r="BD12" s="29"/>
+      <c r="BE12" s="29"/>
+      <c r="BF12" s="29"/>
+      <c r="BG12" s="29"/>
+      <c r="BH12" s="29"/>
+      <c r="BI12" s="29"/>
+      <c r="BJ12" s="29"/>
+      <c r="BK12" s="29"/>
     </row>
     <row r="13" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A13" s="12"/>
       <c r="B13" s="31" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="C13" s="27"/>
       <c r="D13" s="24">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="E13" s="52">
         <v>43895</v>
       </c>
       <c r="F13" s="26">
-        <v>42</v>
+        <v>15</v>
       </c>
       <c r="G13" s="20"/>
       <c r="H13" s="29"/>
@@ -3832,17 +3502,17 @@
     <row r="14" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A14" s="12"/>
       <c r="B14" s="31" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C14" s="27"/>
       <c r="D14" s="24">
-        <v>0</v>
+        <v>0.6</v>
       </c>
       <c r="E14" s="52">
-        <v>43922</v>
+        <v>43895</v>
       </c>
       <c r="F14" s="26">
-        <v>15</v>
+        <v>42</v>
       </c>
       <c r="G14" s="20"/>
       <c r="H14" s="29"/>
@@ -3905,17 +3575,17 @@
     <row r="15" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A15" s="12"/>
       <c r="B15" s="31" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C15" s="27"/>
       <c r="D15" s="24">
         <v>0</v>
       </c>
       <c r="E15" s="52">
-        <v>43936</v>
+        <v>43922</v>
       </c>
       <c r="F15" s="26">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="G15" s="20"/>
       <c r="H15" s="29"/>
@@ -3978,7 +3648,7 @@
     <row r="16" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A16" s="12"/>
       <c r="B16" s="31" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C16" s="27"/>
       <c r="D16" s="24">
@@ -4051,732 +3721,395 @@
     <row r="17" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A17" s="12"/>
       <c r="B17" s="31" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="C17" s="27"/>
       <c r="D17" s="24">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="E17" s="52">
-        <v>43957</v>
+        <v>43936</v>
       </c>
       <c r="F17" s="26">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="G17" s="20"/>
-      <c r="H17" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(H$5=$E17,$F17=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="I17" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(I$5=$E17,$F17=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="J17" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(J$5=$E17,$F17=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="K17" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(K$5=$E17,$F17=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="L17" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(L$5=$E17,$F17=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="M17" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(M$5=$E17,$F17=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="N17" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(N$5=$E17,$F17=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="O17" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(O$5=$E17,$F17=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="P17" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(P$5=$E17,$F17=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="Q17" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(Q$5=$E17,$F17=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="R17" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(R$5=$E17,$F17=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="S17" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(S$5=$E17,$F17=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="T17" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(T$5=$E17,$F17=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="U17" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(U$5=$E17,$F17=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="V17" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(V$5=$E17,$F17=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="W17" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(W$5=$E17,$F17=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="X17" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(X$5=$E17,$F17=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="Y17" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(Y$5=$E17,$F17=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="Z17" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(Z$5=$E17,$F17=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="AA17" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AA$5=$E17,$F17=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="AB17" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AB$5=$E17,$F17=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="AC17" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AC$5=$E17,$F17=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="AD17" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AD$5=$E17,$F17=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="AE17" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AE$5=$E17,$F17=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="AF17" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AF$5=$E17,$F17=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="AG17" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AG$5=$E17,$F17=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="AH17" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AH$5=$E17,$F17=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="AI17" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AI$5=$E17,$F17=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="AJ17" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AJ$5=$E17,$F17=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="AK17" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AK$5=$E17,$F17=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="AL17" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AL$5=$E17,$F17=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="AM17" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AM$5=$E17,$F17=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="AN17" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AN$5=$E17,$F17=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="AO17" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AO$5=$E17,$F17=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="AP17" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AP$5=$E17,$F17=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="AQ17" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AQ$5=$E17,$F17=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="AR17" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AR$5=$E17,$F17=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="AS17" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AS$5=$E17,$F17=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="AT17" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AT$5=$E17,$F17=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="AU17" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AU$5=$E17,$F17=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="AV17" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AV$5=$E17,$F17=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="AW17" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AW$5=$E17,$F17=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="AX17" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AX$5=$E17,$F17=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="AY17" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AY$5=$E17,$F17=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="AZ17" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AZ$5=$E17,$F17=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="BA17" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(BA$5=$E17,$F17=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="BB17" s="29">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(BB$5=$E17,$F17=1),Meilenstein_Markierung,"")),"")</f>
-        <v>1</v>
-      </c>
-      <c r="BC17" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(BC$5=$E17,$F17=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="BD17" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(BD$5=$E17,$F17=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="BE17" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(BE$5=$E17,$F17=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="BF17" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(BF$5=$E17,$F17=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="BG17" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(BG$5=$E17,$F17=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="BH17" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(BH$5=$E17,$F17=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="BI17" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(BI$5=$E17,$F17=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="BJ17" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(BJ$5=$E17,$F17=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="BK17" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(BK$5=$E17,$F17=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
+      <c r="H17" s="29"/>
+      <c r="I17" s="29"/>
+      <c r="J17" s="29"/>
+      <c r="K17" s="29"/>
+      <c r="L17" s="29"/>
+      <c r="M17" s="29"/>
+      <c r="N17" s="29"/>
+      <c r="O17" s="29"/>
+      <c r="P17" s="29"/>
+      <c r="Q17" s="29"/>
+      <c r="R17" s="29"/>
+      <c r="S17" s="29"/>
+      <c r="T17" s="29"/>
+      <c r="U17" s="29"/>
+      <c r="V17" s="29"/>
+      <c r="W17" s="29"/>
+      <c r="X17" s="29"/>
+      <c r="Y17" s="29"/>
+      <c r="Z17" s="29"/>
+      <c r="AA17" s="29"/>
+      <c r="AB17" s="29"/>
+      <c r="AC17" s="29"/>
+      <c r="AD17" s="29"/>
+      <c r="AE17" s="29"/>
+      <c r="AF17" s="29"/>
+      <c r="AG17" s="29"/>
+      <c r="AH17" s="29"/>
+      <c r="AI17" s="29"/>
+      <c r="AJ17" s="29"/>
+      <c r="AK17" s="29"/>
+      <c r="AL17" s="29"/>
+      <c r="AM17" s="29"/>
+      <c r="AN17" s="29"/>
+      <c r="AO17" s="29"/>
+      <c r="AP17" s="29"/>
+      <c r="AQ17" s="29"/>
+      <c r="AR17" s="29"/>
+      <c r="AS17" s="29"/>
+      <c r="AT17" s="29"/>
+      <c r="AU17" s="29"/>
+      <c r="AV17" s="29"/>
+      <c r="AW17" s="29"/>
+      <c r="AX17" s="29"/>
+      <c r="AY17" s="29"/>
+      <c r="AZ17" s="29"/>
+      <c r="BA17" s="29"/>
+      <c r="BB17" s="29"/>
+      <c r="BC17" s="29"/>
+      <c r="BD17" s="29"/>
+      <c r="BE17" s="29"/>
+      <c r="BF17" s="29"/>
+      <c r="BG17" s="29"/>
+      <c r="BH17" s="29"/>
+      <c r="BI17" s="29"/>
+      <c r="BJ17" s="29"/>
+      <c r="BK17" s="29"/>
     </row>
     <row r="18" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A18" s="13"/>
-      <c r="B18" s="59" t="s">
-        <v>33</v>
-      </c>
-      <c r="C18" s="60"/>
-      <c r="D18" s="61"/>
-      <c r="E18" s="62"/>
-      <c r="F18" s="63"/>
+      <c r="A18" s="12"/>
+      <c r="B18" s="31" t="s">
+        <v>36</v>
+      </c>
+      <c r="C18" s="27"/>
+      <c r="D18" s="24">
+        <v>0</v>
+      </c>
+      <c r="E18" s="52">
+        <v>43957</v>
+      </c>
+      <c r="F18" s="26">
+        <v>1</v>
+      </c>
       <c r="G18" s="20"/>
-      <c r="H18" s="29" t="str">
-        <f>IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(H$5=$E18,$F18=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="I18" s="29" t="str">
-        <f>IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(I$5=$E18,$F18=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="J18" s="29" t="str">
-        <f>IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(J$5=$E18,$F18=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="K18" s="29" t="str">
-        <f>IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(K$5=$E18,$F18=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="L18" s="29" t="str">
-        <f>IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(L$5=$E18,$F18=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="M18" s="29" t="str">
-        <f>IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(M$5=$E18,$F18=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="N18" s="29" t="str">
-        <f>IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(N$5=$E18,$F18=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="O18" s="29" t="str">
-        <f>IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(O$5=$E18,$F18=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="P18" s="29" t="str">
-        <f>IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(P$5=$E18,$F18=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="Q18" s="29" t="str">
-        <f>IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(Q$5=$E18,$F18=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="R18" s="29" t="str">
-        <f>IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(R$5=$E18,$F18=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="S18" s="29" t="str">
-        <f>IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(S$5=$E18,$F18=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="T18" s="29" t="str">
-        <f>IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(T$5=$E18,$F18=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="U18" s="29" t="str">
-        <f>IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(U$5=$E18,$F18=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="V18" s="29" t="str">
-        <f>IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(V$5=$E18,$F18=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="W18" s="29" t="str">
-        <f>IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(W$5=$E18,$F18=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="X18" s="29" t="str">
-        <f>IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(X$5=$E18,$F18=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="Y18" s="29" t="str">
-        <f>IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(Y$5=$E18,$F18=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="Z18" s="29" t="str">
-        <f>IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(Z$5=$E18,$F18=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="AA18" s="29" t="str">
-        <f>IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AA$5=$E18,$F18=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="AB18" s="29" t="str">
-        <f>IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AB$5=$E18,$F18=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="AC18" s="29" t="str">
-        <f>IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AC$5=$E18,$F18=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="AD18" s="29" t="str">
-        <f>IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AD$5=$E18,$F18=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="AE18" s="29" t="str">
-        <f>IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AE$5=$E18,$F18=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="AF18" s="29" t="str">
-        <f>IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AF$5=$E18,$F18=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="AG18" s="29" t="str">
-        <f>IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AG$5=$E18,$F18=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="AH18" s="29" t="str">
-        <f>IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AH$5=$E18,$F18=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="AI18" s="29" t="str">
-        <f>IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AI$5=$E18,$F18=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="AJ18" s="29" t="str">
-        <f>IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AJ$5=$E18,$F18=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="AK18" s="29" t="str">
-        <f>IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AK$5=$E18,$F18=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="AL18" s="29" t="str">
-        <f>IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AL$5=$E18,$F18=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="AM18" s="29" t="str">
-        <f>IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AM$5=$E18,$F18=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="AN18" s="29" t="str">
-        <f>IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AN$5=$E18,$F18=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="AO18" s="29" t="str">
-        <f>IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AO$5=$E18,$F18=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="AP18" s="29" t="str">
-        <f>IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AP$5=$E18,$F18=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="AQ18" s="29" t="str">
-        <f>IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AQ$5=$E18,$F18=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="AR18" s="29" t="str">
-        <f>IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AR$5=$E18,$F18=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="AS18" s="29" t="str">
-        <f>IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AS$5=$E18,$F18=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="AT18" s="29" t="str">
-        <f>IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AT$5=$E18,$F18=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="AU18" s="29" t="str">
-        <f>IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AU$5=$E18,$F18=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="AV18" s="29" t="str">
-        <f>IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AV$5=$E18,$F18=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="AW18" s="29" t="str">
-        <f>IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AW$5=$E18,$F18=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="AX18" s="29" t="str">
-        <f>IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AX$5=$E18,$F18=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="AY18" s="29" t="str">
-        <f>IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AY$5=$E18,$F18=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="AZ18" s="29" t="str">
-        <f>IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AZ$5=$E18,$F18=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="BA18" s="29" t="str">
-        <f>IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(BA$5=$E18,$F18=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="BB18" s="29" t="str">
-        <f>IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(BB$5=$E18,$F18=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="BC18" s="29" t="str">
-        <f>IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(BC$5=$E18,$F18=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="BD18" s="29" t="str">
-        <f>IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(BD$5=$E18,$F18=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="BE18" s="29" t="str">
-        <f>IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(BE$5=$E18,$F18=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="BF18" s="29" t="str">
-        <f>IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(BF$5=$E18,$F18=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="BG18" s="29" t="str">
-        <f>IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(BG$5=$E18,$F18=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="BH18" s="29" t="str">
-        <f>IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(BH$5=$E18,$F18=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="BI18" s="29" t="str">
-        <f>IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(BI$5=$E18,$F18=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="BJ18" s="29" t="str">
-        <f>IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(BJ$5=$E18,$F18=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="BK18" s="29" t="str">
-        <f>IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(BK$5=$E18,$F18=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
+      <c r="H18" s="29"/>
+      <c r="I18" s="29"/>
+      <c r="J18" s="29"/>
+      <c r="K18" s="29"/>
+      <c r="L18" s="29"/>
+      <c r="M18" s="29"/>
+      <c r="N18" s="29"/>
+      <c r="O18" s="29"/>
+      <c r="P18" s="29"/>
+      <c r="Q18" s="29"/>
+      <c r="R18" s="29"/>
+      <c r="S18" s="29"/>
+      <c r="T18" s="29"/>
+      <c r="U18" s="29"/>
+      <c r="V18" s="29"/>
+      <c r="W18" s="29"/>
+      <c r="X18" s="29"/>
+      <c r="Y18" s="29"/>
+      <c r="Z18" s="29"/>
+      <c r="AA18" s="29"/>
+      <c r="AB18" s="29"/>
+      <c r="AC18" s="29"/>
+      <c r="AD18" s="29"/>
+      <c r="AE18" s="29"/>
+      <c r="AF18" s="29"/>
+      <c r="AG18" s="29"/>
+      <c r="AH18" s="29"/>
+      <c r="AI18" s="29"/>
+      <c r="AJ18" s="29"/>
+      <c r="AK18" s="29"/>
+      <c r="AL18" s="29"/>
+      <c r="AM18" s="29"/>
+      <c r="AN18" s="29"/>
+      <c r="AO18" s="29"/>
+      <c r="AP18" s="29"/>
+      <c r="AQ18" s="29"/>
+      <c r="AR18" s="29"/>
+      <c r="AS18" s="29"/>
+      <c r="AT18" s="29"/>
+      <c r="AU18" s="29"/>
+      <c r="AV18" s="29"/>
+      <c r="AW18" s="29"/>
+      <c r="AX18" s="29"/>
+      <c r="AY18" s="29"/>
+      <c r="AZ18" s="29"/>
+      <c r="BA18" s="29"/>
+      <c r="BB18" s="29"/>
+      <c r="BC18" s="29"/>
+      <c r="BD18" s="29"/>
+      <c r="BE18" s="29"/>
+      <c r="BF18" s="29"/>
+      <c r="BG18" s="29"/>
+      <c r="BH18" s="29"/>
+      <c r="BI18" s="29"/>
+      <c r="BJ18" s="29"/>
+      <c r="BK18" s="29"/>
     </row>
     <row r="19" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A19" s="13"/>
-      <c r="B19" s="31" t="s">
-        <v>41</v>
-      </c>
-      <c r="C19" s="27"/>
-      <c r="D19" s="24">
-        <v>0.6</v>
-      </c>
-      <c r="E19" s="52">
-        <v>43957</v>
-      </c>
-      <c r="F19" s="26">
-        <v>0</v>
-      </c>
+      <c r="B19" s="53" t="s">
+        <v>28</v>
+      </c>
+      <c r="C19" s="54"/>
+      <c r="D19" s="55"/>
+      <c r="E19" s="56"/>
+      <c r="F19" s="57"/>
       <c r="G19" s="20"/>
       <c r="H19" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(H$5=$E19,$F19=1),Meilenstein_Markierung,"")),"")</f>
+        <f>IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(H$5=$E19,$F19=1),Meilenstein_Markierung,"")),"")</f>
         <v/>
       </c>
       <c r="I19" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(I$5=$E19,$F19=1),Meilenstein_Markierung,"")),"")</f>
+        <f>IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(I$5=$E19,$F19=1),Meilenstein_Markierung,"")),"")</f>
         <v/>
       </c>
       <c r="J19" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(J$5=$E19,$F19=1),Meilenstein_Markierung,"")),"")</f>
+        <f>IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(J$5=$E19,$F19=1),Meilenstein_Markierung,"")),"")</f>
         <v/>
       </c>
       <c r="K19" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(K$5=$E19,$F19=1),Meilenstein_Markierung,"")),"")</f>
+        <f>IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(K$5=$E19,$F19=1),Meilenstein_Markierung,"")),"")</f>
         <v/>
       </c>
       <c r="L19" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(L$5=$E19,$F19=1),Meilenstein_Markierung,"")),"")</f>
+        <f>IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(L$5=$E19,$F19=1),Meilenstein_Markierung,"")),"")</f>
         <v/>
       </c>
       <c r="M19" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(M$5=$E19,$F19=1),Meilenstein_Markierung,"")),"")</f>
+        <f>IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(M$5=$E19,$F19=1),Meilenstein_Markierung,"")),"")</f>
         <v/>
       </c>
       <c r="N19" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(N$5=$E19,$F19=1),Meilenstein_Markierung,"")),"")</f>
+        <f>IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(N$5=$E19,$F19=1),Meilenstein_Markierung,"")),"")</f>
         <v/>
       </c>
       <c r="O19" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(O$5=$E19,$F19=1),Meilenstein_Markierung,"")),"")</f>
+        <f>IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(O$5=$E19,$F19=1),Meilenstein_Markierung,"")),"")</f>
         <v/>
       </c>
       <c r="P19" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(P$5=$E19,$F19=1),Meilenstein_Markierung,"")),"")</f>
+        <f>IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(P$5=$E19,$F19=1),Meilenstein_Markierung,"")),"")</f>
         <v/>
       </c>
       <c r="Q19" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(Q$5=$E19,$F19=1),Meilenstein_Markierung,"")),"")</f>
+        <f>IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(Q$5=$E19,$F19=1),Meilenstein_Markierung,"")),"")</f>
         <v/>
       </c>
       <c r="R19" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(R$5=$E19,$F19=1),Meilenstein_Markierung,"")),"")</f>
+        <f>IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(R$5=$E19,$F19=1),Meilenstein_Markierung,"")),"")</f>
         <v/>
       </c>
       <c r="S19" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(S$5=$E19,$F19=1),Meilenstein_Markierung,"")),"")</f>
+        <f>IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(S$5=$E19,$F19=1),Meilenstein_Markierung,"")),"")</f>
         <v/>
       </c>
       <c r="T19" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(T$5=$E19,$F19=1),Meilenstein_Markierung,"")),"")</f>
+        <f>IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(T$5=$E19,$F19=1),Meilenstein_Markierung,"")),"")</f>
         <v/>
       </c>
       <c r="U19" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(U$5=$E19,$F19=1),Meilenstein_Markierung,"")),"")</f>
+        <f>IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(U$5=$E19,$F19=1),Meilenstein_Markierung,"")),"")</f>
         <v/>
       </c>
       <c r="V19" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(V$5=$E19,$F19=1),Meilenstein_Markierung,"")),"")</f>
+        <f>IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(V$5=$E19,$F19=1),Meilenstein_Markierung,"")),"")</f>
         <v/>
       </c>
       <c r="W19" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(W$5=$E19,$F19=1),Meilenstein_Markierung,"")),"")</f>
+        <f>IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(W$5=$E19,$F19=1),Meilenstein_Markierung,"")),"")</f>
         <v/>
       </c>
       <c r="X19" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(X$5=$E19,$F19=1),Meilenstein_Markierung,"")),"")</f>
+        <f>IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(X$5=$E19,$F19=1),Meilenstein_Markierung,"")),"")</f>
         <v/>
       </c>
       <c r="Y19" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(Y$5=$E19,$F19=1),Meilenstein_Markierung,"")),"")</f>
+        <f>IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(Y$5=$E19,$F19=1),Meilenstein_Markierung,"")),"")</f>
         <v/>
       </c>
       <c r="Z19" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(Z$5=$E19,$F19=1),Meilenstein_Markierung,"")),"")</f>
+        <f>IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(Z$5=$E19,$F19=1),Meilenstein_Markierung,"")),"")</f>
         <v/>
       </c>
       <c r="AA19" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AA$5=$E19,$F19=1),Meilenstein_Markierung,"")),"")</f>
+        <f>IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AA$5=$E19,$F19=1),Meilenstein_Markierung,"")),"")</f>
         <v/>
       </c>
       <c r="AB19" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AB$5=$E19,$F19=1),Meilenstein_Markierung,"")),"")</f>
+        <f>IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AB$5=$E19,$F19=1),Meilenstein_Markierung,"")),"")</f>
         <v/>
       </c>
       <c r="AC19" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AC$5=$E19,$F19=1),Meilenstein_Markierung,"")),"")</f>
+        <f>IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AC$5=$E19,$F19=1),Meilenstein_Markierung,"")),"")</f>
         <v/>
       </c>
       <c r="AD19" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AD$5=$E19,$F19=1),Meilenstein_Markierung,"")),"")</f>
+        <f>IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AD$5=$E19,$F19=1),Meilenstein_Markierung,"")),"")</f>
         <v/>
       </c>
       <c r="AE19" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AE$5=$E19,$F19=1),Meilenstein_Markierung,"")),"")</f>
+        <f>IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AE$5=$E19,$F19=1),Meilenstein_Markierung,"")),"")</f>
         <v/>
       </c>
       <c r="AF19" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AF$5=$E19,$F19=1),Meilenstein_Markierung,"")),"")</f>
+        <f>IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AF$5=$E19,$F19=1),Meilenstein_Markierung,"")),"")</f>
         <v/>
       </c>
       <c r="AG19" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AG$5=$E19,$F19=1),Meilenstein_Markierung,"")),"")</f>
+        <f>IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AG$5=$E19,$F19=1),Meilenstein_Markierung,"")),"")</f>
         <v/>
       </c>
       <c r="AH19" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AH$5=$E19,$F19=1),Meilenstein_Markierung,"")),"")</f>
+        <f>IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AH$5=$E19,$F19=1),Meilenstein_Markierung,"")),"")</f>
         <v/>
       </c>
       <c r="AI19" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AI$5=$E19,$F19=1),Meilenstein_Markierung,"")),"")</f>
+        <f>IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AI$5=$E19,$F19=1),Meilenstein_Markierung,"")),"")</f>
         <v/>
       </c>
       <c r="AJ19" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AJ$5=$E19,$F19=1),Meilenstein_Markierung,"")),"")</f>
+        <f>IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AJ$5=$E19,$F19=1),Meilenstein_Markierung,"")),"")</f>
         <v/>
       </c>
       <c r="AK19" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AK$5=$E19,$F19=1),Meilenstein_Markierung,"")),"")</f>
+        <f>IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AK$5=$E19,$F19=1),Meilenstein_Markierung,"")),"")</f>
         <v/>
       </c>
       <c r="AL19" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AL$5=$E19,$F19=1),Meilenstein_Markierung,"")),"")</f>
+        <f>IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AL$5=$E19,$F19=1),Meilenstein_Markierung,"")),"")</f>
         <v/>
       </c>
       <c r="AM19" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AM$5=$E19,$F19=1),Meilenstein_Markierung,"")),"")</f>
+        <f>IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AM$5=$E19,$F19=1),Meilenstein_Markierung,"")),"")</f>
         <v/>
       </c>
       <c r="AN19" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AN$5=$E19,$F19=1),Meilenstein_Markierung,"")),"")</f>
+        <f>IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AN$5=$E19,$F19=1),Meilenstein_Markierung,"")),"")</f>
         <v/>
       </c>
       <c r="AO19" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AO$5=$E19,$F19=1),Meilenstein_Markierung,"")),"")</f>
+        <f>IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AO$5=$E19,$F19=1),Meilenstein_Markierung,"")),"")</f>
         <v/>
       </c>
       <c r="AP19" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AP$5=$E19,$F19=1),Meilenstein_Markierung,"")),"")</f>
+        <f>IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AP$5=$E19,$F19=1),Meilenstein_Markierung,"")),"")</f>
         <v/>
       </c>
       <c r="AQ19" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AQ$5=$E19,$F19=1),Meilenstein_Markierung,"")),"")</f>
+        <f>IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AQ$5=$E19,$F19=1),Meilenstein_Markierung,"")),"")</f>
         <v/>
       </c>
       <c r="AR19" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AR$5=$E19,$F19=1),Meilenstein_Markierung,"")),"")</f>
+        <f>IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AR$5=$E19,$F19=1),Meilenstein_Markierung,"")),"")</f>
         <v/>
       </c>
       <c r="AS19" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AS$5=$E19,$F19=1),Meilenstein_Markierung,"")),"")</f>
+        <f>IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AS$5=$E19,$F19=1),Meilenstein_Markierung,"")),"")</f>
         <v/>
       </c>
       <c r="AT19" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AT$5=$E19,$F19=1),Meilenstein_Markierung,"")),"")</f>
+        <f>IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AT$5=$E19,$F19=1),Meilenstein_Markierung,"")),"")</f>
         <v/>
       </c>
       <c r="AU19" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AU$5=$E19,$F19=1),Meilenstein_Markierung,"")),"")</f>
+        <f>IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AU$5=$E19,$F19=1),Meilenstein_Markierung,"")),"")</f>
         <v/>
       </c>
       <c r="AV19" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AV$5=$E19,$F19=1),Meilenstein_Markierung,"")),"")</f>
+        <f>IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AV$5=$E19,$F19=1),Meilenstein_Markierung,"")),"")</f>
         <v/>
       </c>
       <c r="AW19" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AW$5=$E19,$F19=1),Meilenstein_Markierung,"")),"")</f>
+        <f>IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AW$5=$E19,$F19=1),Meilenstein_Markierung,"")),"")</f>
         <v/>
       </c>
       <c r="AX19" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AX$5=$E19,$F19=1),Meilenstein_Markierung,"")),"")</f>
+        <f>IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AX$5=$E19,$F19=1),Meilenstein_Markierung,"")),"")</f>
         <v/>
       </c>
       <c r="AY19" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AY$5=$E19,$F19=1),Meilenstein_Markierung,"")),"")</f>
+        <f>IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AY$5=$E19,$F19=1),Meilenstein_Markierung,"")),"")</f>
         <v/>
       </c>
       <c r="AZ19" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AZ$5=$E19,$F19=1),Meilenstein_Markierung,"")),"")</f>
+        <f>IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AZ$5=$E19,$F19=1),Meilenstein_Markierung,"")),"")</f>
         <v/>
       </c>
       <c r="BA19" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(BA$5=$E19,$F19=1),Meilenstein_Markierung,"")),"")</f>
+        <f>IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(BA$5=$E19,$F19=1),Meilenstein_Markierung,"")),"")</f>
         <v/>
       </c>
       <c r="BB19" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(BB$5=$E19,$F19=1),Meilenstein_Markierung,"")),"")</f>
+        <f>IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(BB$5=$E19,$F19=1),Meilenstein_Markierung,"")),"")</f>
         <v/>
       </c>
       <c r="BC19" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(BC$5=$E19,$F19=1),Meilenstein_Markierung,"")),"")</f>
+        <f>IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(BC$5=$E19,$F19=1),Meilenstein_Markierung,"")),"")</f>
         <v/>
       </c>
       <c r="BD19" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(BD$5=$E19,$F19=1),Meilenstein_Markierung,"")),"")</f>
+        <f>IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(BD$5=$E19,$F19=1),Meilenstein_Markierung,"")),"")</f>
         <v/>
       </c>
       <c r="BE19" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(BE$5=$E19,$F19=1),Meilenstein_Markierung,"")),"")</f>
+        <f>IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(BE$5=$E19,$F19=1),Meilenstein_Markierung,"")),"")</f>
         <v/>
       </c>
       <c r="BF19" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(BF$5=$E19,$F19=1),Meilenstein_Markierung,"")),"")</f>
+        <f>IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(BF$5=$E19,$F19=1),Meilenstein_Markierung,"")),"")</f>
         <v/>
       </c>
       <c r="BG19" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(BG$5=$E19,$F19=1),Meilenstein_Markierung,"")),"")</f>
+        <f>IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(BG$5=$E19,$F19=1),Meilenstein_Markierung,"")),"")</f>
         <v/>
       </c>
       <c r="BH19" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(BH$5=$E19,$F19=1),Meilenstein_Markierung,"")),"")</f>
+        <f>IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(BH$5=$E19,$F19=1),Meilenstein_Markierung,"")),"")</f>
         <v/>
       </c>
       <c r="BI19" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(BI$5=$E19,$F19=1),Meilenstein_Markierung,"")),"")</f>
+        <f>IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(BI$5=$E19,$F19=1),Meilenstein_Markierung,"")),"")</f>
         <v/>
       </c>
       <c r="BJ19" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(BJ$5=$E19,$F19=1),Meilenstein_Markierung,"")),"")</f>
+        <f>IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(BJ$5=$E19,$F19=1),Meilenstein_Markierung,"")),"")</f>
         <v/>
       </c>
       <c r="BK19" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(BK$5=$E19,$F19=1),Meilenstein_Markierung,"")),"")</f>
+        <f>IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(BK$5=$E19,$F19=1),Meilenstein_Markierung,"")),"")</f>
         <v/>
       </c>
     </row>
     <row r="20" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A20" s="12"/>
+      <c r="A20" s="13"/>
       <c r="B20" s="31" t="s">
-        <v>11</v>
+        <v>33</v>
       </c>
       <c r="C20" s="27"/>
       <c r="D20" s="24">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="E20" s="52">
-        <f ca="1">TODAY()+7</f>
-        <v>43928</v>
+        <v>43957</v>
       </c>
       <c r="F20" s="26">
         <v>0</v>
@@ -5010,15 +4343,15 @@
     <row r="21" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A21" s="12"/>
       <c r="B21" s="31" t="s">
-        <v>12</v>
+        <v>38</v>
       </c>
       <c r="C21" s="27"/>
       <c r="D21" s="24">
-        <v>0.33</v>
+        <v>0</v>
       </c>
       <c r="E21" s="52">
-        <f ca="1">TODAY()+15</f>
-        <v>43936</v>
+        <f ca="1">TODAY()+7</f>
+        <v>43928</v>
       </c>
       <c r="F21" s="26">
         <v>0</v>
@@ -5252,13 +4585,15 @@
     <row r="22" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A22" s="12"/>
       <c r="B22" s="31" t="s">
-        <v>13</v>
+        <v>40</v>
       </c>
       <c r="C22" s="27"/>
-      <c r="D22" s="24"/>
+      <c r="D22" s="24">
+        <v>0</v>
+      </c>
       <c r="E22" s="52">
-        <f ca="1">TODAY()+24</f>
-        <v>43945</v>
+        <f ca="1">TODAY()+15</f>
+        <v>43936</v>
       </c>
       <c r="F22" s="26">
         <v>0</v>
@@ -5492,15 +4827,17 @@
     <row r="23" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A23" s="12"/>
       <c r="B23" s="31" t="s">
-        <v>14</v>
+        <v>35</v>
       </c>
       <c r="C23" s="27"/>
-      <c r="D23" s="24"/>
+      <c r="D23" s="24">
+        <v>0</v>
+      </c>
       <c r="E23" s="52">
         <v>43985</v>
       </c>
       <c r="F23" s="26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G23" s="20"/>
       <c r="H23" s="29" t="str">
@@ -5730,13 +5067,13 @@
     </row>
     <row r="24" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A24" s="12"/>
-      <c r="B24" s="59" t="s">
-        <v>34</v>
-      </c>
-      <c r="C24" s="60"/>
-      <c r="D24" s="61"/>
-      <c r="E24" s="62"/>
-      <c r="F24" s="63"/>
+      <c r="B24" s="53" t="s">
+        <v>29</v>
+      </c>
+      <c r="C24" s="54"/>
+      <c r="D24" s="55"/>
+      <c r="E24" s="56"/>
+      <c r="F24" s="57"/>
       <c r="G24" s="20"/>
       <c r="H24" s="29" t="str">
         <f>IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(H$5=$E24,$F24=1),Meilenstein_Markierung,"")),"")</f>
@@ -5966,10 +5303,12 @@
     <row r="25" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A25" s="12"/>
       <c r="B25" s="31" t="s">
-        <v>10</v>
+        <v>42</v>
       </c>
       <c r="C25" s="27"/>
-      <c r="D25" s="24"/>
+      <c r="D25" s="24">
+        <v>0</v>
+      </c>
       <c r="E25" s="52">
         <v>43985</v>
       </c>
@@ -6205,13 +5544,14 @@
     <row r="26" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A26" s="12"/>
       <c r="B26" s="31" t="s">
-        <v>11</v>
+        <v>44</v>
       </c>
       <c r="C26" s="27"/>
-      <c r="D26" s="24"/>
+      <c r="D26" s="24">
+        <v>0</v>
+      </c>
       <c r="E26" s="52">
-        <f ca="1">TODAY()+19</f>
-        <v>43940</v>
+        <v>43992</v>
       </c>
       <c r="F26" s="26">
         <v>0</v>
@@ -6445,13 +5785,14 @@
     <row r="27" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A27" s="12"/>
       <c r="B27" s="31" t="s">
-        <v>12</v>
+        <v>43</v>
       </c>
       <c r="C27" s="27"/>
-      <c r="D27" s="24"/>
+      <c r="D27" s="24">
+        <v>0</v>
+      </c>
       <c r="E27" s="52">
-        <f ca="1">TODAY()+35</f>
-        <v>43956</v>
+        <v>43992</v>
       </c>
       <c r="F27" s="26">
         <v>0</v>
@@ -6685,13 +6026,14 @@
     <row r="28" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A28" s="12"/>
       <c r="B28" s="31" t="s">
-        <v>13</v>
+        <v>45</v>
       </c>
       <c r="C28" s="27"/>
-      <c r="D28" s="24"/>
+      <c r="D28" s="24">
+        <v>0</v>
+      </c>
       <c r="E28" s="52">
-        <f ca="1">TODAY()+48</f>
-        <v>43969</v>
+        <v>44013</v>
       </c>
       <c r="F28" s="26">
         <v>0</v>
@@ -6925,553 +6267,628 @@
     <row r="29" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A29" s="12"/>
       <c r="B29" s="31" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="C29" s="27"/>
-      <c r="D29" s="24"/>
+      <c r="D29" s="24">
+        <v>0</v>
+      </c>
       <c r="E29" s="52">
-        <v>44048</v>
+        <v>44020</v>
       </c>
       <c r="F29" s="26">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G29" s="20"/>
-      <c r="H29" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(H$5=$E29,$F29=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="I29" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(I$5=$E29,$F29=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="J29" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(J$5=$E29,$F29=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="K29" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(K$5=$E29,$F29=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="L29" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(L$5=$E29,$F29=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="M29" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(M$5=$E29,$F29=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="N29" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(N$5=$E29,$F29=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="O29" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(O$5=$E29,$F29=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="P29" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(P$5=$E29,$F29=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="Q29" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(Q$5=$E29,$F29=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="R29" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(R$5=$E29,$F29=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="S29" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(S$5=$E29,$F29=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="T29" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(T$5=$E29,$F29=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="U29" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(U$5=$E29,$F29=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="V29" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(V$5=$E29,$F29=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="W29" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(W$5=$E29,$F29=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="X29" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(X$5=$E29,$F29=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="Y29" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(Y$5=$E29,$F29=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="Z29" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(Z$5=$E29,$F29=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="AA29" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AA$5=$E29,$F29=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="AB29" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AB$5=$E29,$F29=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="AC29" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AC$5=$E29,$F29=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="AD29" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AD$5=$E29,$F29=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="AE29" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AE$5=$E29,$F29=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="AF29" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AF$5=$E29,$F29=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="AG29" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AG$5=$E29,$F29=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="AH29" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AH$5=$E29,$F29=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="AI29" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AI$5=$E29,$F29=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="AJ29" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AJ$5=$E29,$F29=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="AK29" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AK$5=$E29,$F29=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="AL29" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AL$5=$E29,$F29=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="AM29" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AM$5=$E29,$F29=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="AN29" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AN$5=$E29,$F29=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="AO29" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AO$5=$E29,$F29=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="AP29" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AP$5=$E29,$F29=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="AQ29" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AQ$5=$E29,$F29=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="AR29" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AR$5=$E29,$F29=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="AS29" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AS$5=$E29,$F29=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="AT29" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AT$5=$E29,$F29=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="AU29" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AU$5=$E29,$F29=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="AV29" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AV$5=$E29,$F29=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="AW29" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AW$5=$E29,$F29=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="AX29" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AX$5=$E29,$F29=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="AY29" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AY$5=$E29,$F29=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="AZ29" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AZ$5=$E29,$F29=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="BA29" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(BA$5=$E29,$F29=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="BB29" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(BB$5=$E29,$F29=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="BC29" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(BC$5=$E29,$F29=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="BD29" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(BD$5=$E29,$F29=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="BE29" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(BE$5=$E29,$F29=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="BF29" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(BF$5=$E29,$F29=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="BG29" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(BG$5=$E29,$F29=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="BH29" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(BH$5=$E29,$F29=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="BI29" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(BI$5=$E29,$F29=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="BJ29" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(BJ$5=$E29,$F29=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
-      <c r="BK29" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(BK$5=$E29,$F29=1),Meilenstein_Markierung,"")),"")</f>
-        <v/>
-      </c>
+      <c r="H29" s="29"/>
+      <c r="I29" s="29"/>
+      <c r="J29" s="29"/>
+      <c r="K29" s="29"/>
+      <c r="L29" s="29"/>
+      <c r="M29" s="29"/>
+      <c r="N29" s="29"/>
+      <c r="O29" s="29"/>
+      <c r="P29" s="29"/>
+      <c r="Q29" s="29"/>
+      <c r="R29" s="29"/>
+      <c r="S29" s="29"/>
+      <c r="T29" s="29"/>
+      <c r="U29" s="29"/>
+      <c r="V29" s="29"/>
+      <c r="W29" s="29"/>
+      <c r="X29" s="29"/>
+      <c r="Y29" s="29"/>
+      <c r="Z29" s="29"/>
+      <c r="AA29" s="29"/>
+      <c r="AB29" s="29"/>
+      <c r="AC29" s="29"/>
+      <c r="AD29" s="29"/>
+      <c r="AE29" s="29"/>
+      <c r="AF29" s="29"/>
+      <c r="AG29" s="29"/>
+      <c r="AH29" s="29"/>
+      <c r="AI29" s="29"/>
+      <c r="AJ29" s="29"/>
+      <c r="AK29" s="29"/>
+      <c r="AL29" s="29"/>
+      <c r="AM29" s="29"/>
+      <c r="AN29" s="29"/>
+      <c r="AO29" s="29"/>
+      <c r="AP29" s="29"/>
+      <c r="AQ29" s="29"/>
+      <c r="AR29" s="29"/>
+      <c r="AS29" s="29"/>
+      <c r="AT29" s="29"/>
+      <c r="AU29" s="29"/>
+      <c r="AV29" s="29"/>
+      <c r="AW29" s="29"/>
+      <c r="AX29" s="29"/>
+      <c r="AY29" s="29"/>
+      <c r="AZ29" s="29"/>
+      <c r="BA29" s="29"/>
+      <c r="BB29" s="29"/>
+      <c r="BC29" s="29"/>
+      <c r="BD29" s="29"/>
+      <c r="BE29" s="29"/>
+      <c r="BF29" s="29"/>
+      <c r="BG29" s="29"/>
+      <c r="BH29" s="29"/>
+      <c r="BI29" s="29"/>
+      <c r="BJ29" s="29"/>
+      <c r="BK29" s="29"/>
     </row>
     <row r="30" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A30" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="B30" s="31"/>
+      <c r="A30" s="12"/>
+      <c r="B30" s="31" t="s">
+        <v>37</v>
+      </c>
       <c r="C30" s="27"/>
-      <c r="D30" s="24"/>
-      <c r="E30" s="52"/>
-      <c r="F30" s="26"/>
+      <c r="D30" s="24">
+        <v>0</v>
+      </c>
+      <c r="E30" s="52">
+        <v>44048</v>
+      </c>
+      <c r="F30" s="26">
+        <v>1</v>
+      </c>
       <c r="G30" s="20"/>
       <c r="H30" s="29" t="str">
-        <f>IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(H$5=$E30,$F30=1),Meilenstein_Markierung,"")),"")</f>
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(H$5=$E30,$F30=1),Meilenstein_Markierung,"")),"")</f>
         <v/>
       </c>
       <c r="I30" s="29" t="str">
-        <f>IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(I$5=$E30,$F30=1),Meilenstein_Markierung,"")),"")</f>
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(I$5=$E30,$F30=1),Meilenstein_Markierung,"")),"")</f>
         <v/>
       </c>
       <c r="J30" s="29" t="str">
-        <f>IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(J$5=$E30,$F30=1),Meilenstein_Markierung,"")),"")</f>
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(J$5=$E30,$F30=1),Meilenstein_Markierung,"")),"")</f>
         <v/>
       </c>
       <c r="K30" s="29" t="str">
-        <f>IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(K$5=$E30,$F30=1),Meilenstein_Markierung,"")),"")</f>
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(K$5=$E30,$F30=1),Meilenstein_Markierung,"")),"")</f>
         <v/>
       </c>
       <c r="L30" s="29" t="str">
-        <f>IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(L$5=$E30,$F30=1),Meilenstein_Markierung,"")),"")</f>
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(L$5=$E30,$F30=1),Meilenstein_Markierung,"")),"")</f>
         <v/>
       </c>
       <c r="M30" s="29" t="str">
-        <f>IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(M$5=$E30,$F30=1),Meilenstein_Markierung,"")),"")</f>
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(M$5=$E30,$F30=1),Meilenstein_Markierung,"")),"")</f>
         <v/>
       </c>
       <c r="N30" s="29" t="str">
-        <f>IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(N$5=$E30,$F30=1),Meilenstein_Markierung,"")),"")</f>
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(N$5=$E30,$F30=1),Meilenstein_Markierung,"")),"")</f>
         <v/>
       </c>
       <c r="O30" s="29" t="str">
-        <f>IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(O$5=$E30,$F30=1),Meilenstein_Markierung,"")),"")</f>
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(O$5=$E30,$F30=1),Meilenstein_Markierung,"")),"")</f>
         <v/>
       </c>
       <c r="P30" s="29" t="str">
-        <f>IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(P$5=$E30,$F30=1),Meilenstein_Markierung,"")),"")</f>
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(P$5=$E30,$F30=1),Meilenstein_Markierung,"")),"")</f>
         <v/>
       </c>
       <c r="Q30" s="29" t="str">
-        <f>IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(Q$5=$E30,$F30=1),Meilenstein_Markierung,"")),"")</f>
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(Q$5=$E30,$F30=1),Meilenstein_Markierung,"")),"")</f>
         <v/>
       </c>
       <c r="R30" s="29" t="str">
-        <f>IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(R$5=$E30,$F30=1),Meilenstein_Markierung,"")),"")</f>
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(R$5=$E30,$F30=1),Meilenstein_Markierung,"")),"")</f>
         <v/>
       </c>
       <c r="S30" s="29" t="str">
-        <f>IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(S$5=$E30,$F30=1),Meilenstein_Markierung,"")),"")</f>
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(S$5=$E30,$F30=1),Meilenstein_Markierung,"")),"")</f>
         <v/>
       </c>
       <c r="T30" s="29" t="str">
-        <f>IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(T$5=$E30,$F30=1),Meilenstein_Markierung,"")),"")</f>
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(T$5=$E30,$F30=1),Meilenstein_Markierung,"")),"")</f>
         <v/>
       </c>
       <c r="U30" s="29" t="str">
-        <f>IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(U$5=$E30,$F30=1),Meilenstein_Markierung,"")),"")</f>
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(U$5=$E30,$F30=1),Meilenstein_Markierung,"")),"")</f>
         <v/>
       </c>
       <c r="V30" s="29" t="str">
-        <f>IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(V$5=$E30,$F30=1),Meilenstein_Markierung,"")),"")</f>
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(V$5=$E30,$F30=1),Meilenstein_Markierung,"")),"")</f>
         <v/>
       </c>
       <c r="W30" s="29" t="str">
-        <f>IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(W$5=$E30,$F30=1),Meilenstein_Markierung,"")),"")</f>
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(W$5=$E30,$F30=1),Meilenstein_Markierung,"")),"")</f>
         <v/>
       </c>
       <c r="X30" s="29" t="str">
-        <f>IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(X$5=$E30,$F30=1),Meilenstein_Markierung,"")),"")</f>
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(X$5=$E30,$F30=1),Meilenstein_Markierung,"")),"")</f>
         <v/>
       </c>
       <c r="Y30" s="29" t="str">
-        <f>IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(Y$5=$E30,$F30=1),Meilenstein_Markierung,"")),"")</f>
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(Y$5=$E30,$F30=1),Meilenstein_Markierung,"")),"")</f>
         <v/>
       </c>
       <c r="Z30" s="29" t="str">
-        <f>IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(Z$5=$E30,$F30=1),Meilenstein_Markierung,"")),"")</f>
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(Z$5=$E30,$F30=1),Meilenstein_Markierung,"")),"")</f>
         <v/>
       </c>
       <c r="AA30" s="29" t="str">
-        <f>IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AA$5=$E30,$F30=1),Meilenstein_Markierung,"")),"")</f>
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AA$5=$E30,$F30=1),Meilenstein_Markierung,"")),"")</f>
         <v/>
       </c>
       <c r="AB30" s="29" t="str">
-        <f>IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AB$5=$E30,$F30=1),Meilenstein_Markierung,"")),"")</f>
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AB$5=$E30,$F30=1),Meilenstein_Markierung,"")),"")</f>
         <v/>
       </c>
       <c r="AC30" s="29" t="str">
-        <f>IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AC$5=$E30,$F30=1),Meilenstein_Markierung,"")),"")</f>
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AC$5=$E30,$F30=1),Meilenstein_Markierung,"")),"")</f>
         <v/>
       </c>
       <c r="AD30" s="29" t="str">
-        <f>IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AD$5=$E30,$F30=1),Meilenstein_Markierung,"")),"")</f>
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AD$5=$E30,$F30=1),Meilenstein_Markierung,"")),"")</f>
         <v/>
       </c>
       <c r="AE30" s="29" t="str">
-        <f>IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AE$5=$E30,$F30=1),Meilenstein_Markierung,"")),"")</f>
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AE$5=$E30,$F30=1),Meilenstein_Markierung,"")),"")</f>
         <v/>
       </c>
       <c r="AF30" s="29" t="str">
-        <f>IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AF$5=$E30,$F30=1),Meilenstein_Markierung,"")),"")</f>
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AF$5=$E30,$F30=1),Meilenstein_Markierung,"")),"")</f>
         <v/>
       </c>
       <c r="AG30" s="29" t="str">
-        <f>IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AG$5=$E30,$F30=1),Meilenstein_Markierung,"")),"")</f>
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AG$5=$E30,$F30=1),Meilenstein_Markierung,"")),"")</f>
         <v/>
       </c>
       <c r="AH30" s="29" t="str">
-        <f>IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AH$5=$E30,$F30=1),Meilenstein_Markierung,"")),"")</f>
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AH$5=$E30,$F30=1),Meilenstein_Markierung,"")),"")</f>
         <v/>
       </c>
       <c r="AI30" s="29" t="str">
-        <f>IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AI$5=$E30,$F30=1),Meilenstein_Markierung,"")),"")</f>
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AI$5=$E30,$F30=1),Meilenstein_Markierung,"")),"")</f>
         <v/>
       </c>
       <c r="AJ30" s="29" t="str">
-        <f>IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AJ$5=$E30,$F30=1),Meilenstein_Markierung,"")),"")</f>
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AJ$5=$E30,$F30=1),Meilenstein_Markierung,"")),"")</f>
         <v/>
       </c>
       <c r="AK30" s="29" t="str">
-        <f>IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AK$5=$E30,$F30=1),Meilenstein_Markierung,"")),"")</f>
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AK$5=$E30,$F30=1),Meilenstein_Markierung,"")),"")</f>
         <v/>
       </c>
       <c r="AL30" s="29" t="str">
-        <f>IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AL$5=$E30,$F30=1),Meilenstein_Markierung,"")),"")</f>
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AL$5=$E30,$F30=1),Meilenstein_Markierung,"")),"")</f>
         <v/>
       </c>
       <c r="AM30" s="29" t="str">
-        <f>IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AM$5=$E30,$F30=1),Meilenstein_Markierung,"")),"")</f>
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AM$5=$E30,$F30=1),Meilenstein_Markierung,"")),"")</f>
         <v/>
       </c>
       <c r="AN30" s="29" t="str">
-        <f>IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AN$5=$E30,$F30=1),Meilenstein_Markierung,"")),"")</f>
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AN$5=$E30,$F30=1),Meilenstein_Markierung,"")),"")</f>
         <v/>
       </c>
       <c r="AO30" s="29" t="str">
-        <f>IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AO$5=$E30,$F30=1),Meilenstein_Markierung,"")),"")</f>
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AO$5=$E30,$F30=1),Meilenstein_Markierung,"")),"")</f>
         <v/>
       </c>
       <c r="AP30" s="29" t="str">
-        <f>IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AP$5=$E30,$F30=1),Meilenstein_Markierung,"")),"")</f>
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AP$5=$E30,$F30=1),Meilenstein_Markierung,"")),"")</f>
         <v/>
       </c>
       <c r="AQ30" s="29" t="str">
-        <f>IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AQ$5=$E30,$F30=1),Meilenstein_Markierung,"")),"")</f>
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AQ$5=$E30,$F30=1),Meilenstein_Markierung,"")),"")</f>
         <v/>
       </c>
       <c r="AR30" s="29" t="str">
-        <f>IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AR$5=$E30,$F30=1),Meilenstein_Markierung,"")),"")</f>
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AR$5=$E30,$F30=1),Meilenstein_Markierung,"")),"")</f>
         <v/>
       </c>
       <c r="AS30" s="29" t="str">
-        <f>IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AS$5=$E30,$F30=1),Meilenstein_Markierung,"")),"")</f>
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AS$5=$E30,$F30=1),Meilenstein_Markierung,"")),"")</f>
         <v/>
       </c>
       <c r="AT30" s="29" t="str">
-        <f>IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AT$5=$E30,$F30=1),Meilenstein_Markierung,"")),"")</f>
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AT$5=$E30,$F30=1),Meilenstein_Markierung,"")),"")</f>
         <v/>
       </c>
       <c r="AU30" s="29" t="str">
-        <f>IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AU$5=$E30,$F30=1),Meilenstein_Markierung,"")),"")</f>
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AU$5=$E30,$F30=1),Meilenstein_Markierung,"")),"")</f>
         <v/>
       </c>
       <c r="AV30" s="29" t="str">
-        <f>IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AV$5=$E30,$F30=1),Meilenstein_Markierung,"")),"")</f>
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AV$5=$E30,$F30=1),Meilenstein_Markierung,"")),"")</f>
         <v/>
       </c>
       <c r="AW30" s="29" t="str">
-        <f>IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AW$5=$E30,$F30=1),Meilenstein_Markierung,"")),"")</f>
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AW$5=$E30,$F30=1),Meilenstein_Markierung,"")),"")</f>
         <v/>
       </c>
       <c r="AX30" s="29" t="str">
-        <f>IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AX$5=$E30,$F30=1),Meilenstein_Markierung,"")),"")</f>
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AX$5=$E30,$F30=1),Meilenstein_Markierung,"")),"")</f>
         <v/>
       </c>
       <c r="AY30" s="29" t="str">
-        <f>IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AY$5=$E30,$F30=1),Meilenstein_Markierung,"")),"")</f>
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AY$5=$E30,$F30=1),Meilenstein_Markierung,"")),"")</f>
         <v/>
       </c>
       <c r="AZ30" s="29" t="str">
-        <f>IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AZ$5=$E30,$F30=1),Meilenstein_Markierung,"")),"")</f>
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AZ$5=$E30,$F30=1),Meilenstein_Markierung,"")),"")</f>
         <v/>
       </c>
       <c r="BA30" s="29" t="str">
-        <f>IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(BA$5=$E30,$F30=1),Meilenstein_Markierung,"")),"")</f>
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(BA$5=$E30,$F30=1),Meilenstein_Markierung,"")),"")</f>
         <v/>
       </c>
       <c r="BB30" s="29" t="str">
-        <f>IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(BB$5=$E30,$F30=1),Meilenstein_Markierung,"")),"")</f>
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(BB$5=$E30,$F30=1),Meilenstein_Markierung,"")),"")</f>
         <v/>
       </c>
       <c r="BC30" s="29" t="str">
-        <f>IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(BC$5=$E30,$F30=1),Meilenstein_Markierung,"")),"")</f>
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(BC$5=$E30,$F30=1),Meilenstein_Markierung,"")),"")</f>
         <v/>
       </c>
       <c r="BD30" s="29" t="str">
-        <f>IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(BD$5=$E30,$F30=1),Meilenstein_Markierung,"")),"")</f>
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(BD$5=$E30,$F30=1),Meilenstein_Markierung,"")),"")</f>
         <v/>
       </c>
       <c r="BE30" s="29" t="str">
-        <f>IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(BE$5=$E30,$F30=1),Meilenstein_Markierung,"")),"")</f>
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(BE$5=$E30,$F30=1),Meilenstein_Markierung,"")),"")</f>
         <v/>
       </c>
       <c r="BF30" s="29" t="str">
-        <f>IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(BF$5=$E30,$F30=1),Meilenstein_Markierung,"")),"")</f>
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(BF$5=$E30,$F30=1),Meilenstein_Markierung,"")),"")</f>
         <v/>
       </c>
       <c r="BG30" s="29" t="str">
-        <f>IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(BG$5=$E30,$F30=1),Meilenstein_Markierung,"")),"")</f>
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(BG$5=$E30,$F30=1),Meilenstein_Markierung,"")),"")</f>
         <v/>
       </c>
       <c r="BH30" s="29" t="str">
-        <f>IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(BH$5=$E30,$F30=1),Meilenstein_Markierung,"")),"")</f>
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(BH$5=$E30,$F30=1),Meilenstein_Markierung,"")),"")</f>
         <v/>
       </c>
       <c r="BI30" s="29" t="str">
-        <f>IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(BI$5=$E30,$F30=1),Meilenstein_Markierung,"")),"")</f>
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(BI$5=$E30,$F30=1),Meilenstein_Markierung,"")),"")</f>
         <v/>
       </c>
       <c r="BJ30" s="29" t="str">
-        <f>IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(BJ$5=$E30,$F30=1),Meilenstein_Markierung,"")),"")</f>
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(BJ$5=$E30,$F30=1),Meilenstein_Markierung,"")),"")</f>
         <v/>
       </c>
       <c r="BK30" s="29" t="str">
-        <f>IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(BK$5=$E30,$F30=1),Meilenstein_Markierung,"")),"")</f>
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(BK$5=$E30,$F30=1),Meilenstein_Markierung,"")),"")</f>
         <v/>
       </c>
     </row>
-    <row r="31" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A31" s="13" t="s">
+    <row r="31" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A31" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="B31" s="31"/>
+      <c r="C31" s="27"/>
+      <c r="D31" s="24"/>
+      <c r="E31" s="52"/>
+      <c r="F31" s="26"/>
+      <c r="G31" s="20"/>
+      <c r="H31" s="29" t="str">
+        <f>IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(H$5=$E31,$F31=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="I31" s="29" t="str">
+        <f>IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(I$5=$E31,$F31=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="J31" s="29" t="str">
+        <f>IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(J$5=$E31,$F31=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="K31" s="29" t="str">
+        <f>IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(K$5=$E31,$F31=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="L31" s="29" t="str">
+        <f>IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(L$5=$E31,$F31=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="M31" s="29" t="str">
+        <f>IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(M$5=$E31,$F31=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="N31" s="29" t="str">
+        <f>IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(N$5=$E31,$F31=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="O31" s="29" t="str">
+        <f>IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(O$5=$E31,$F31=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="P31" s="29" t="str">
+        <f>IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(P$5=$E31,$F31=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="Q31" s="29" t="str">
+        <f>IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(Q$5=$E31,$F31=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="R31" s="29" t="str">
+        <f>IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(R$5=$E31,$F31=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="S31" s="29" t="str">
+        <f>IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(S$5=$E31,$F31=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="T31" s="29" t="str">
+        <f>IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(T$5=$E31,$F31=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="U31" s="29" t="str">
+        <f>IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(U$5=$E31,$F31=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="V31" s="29" t="str">
+        <f>IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(V$5=$E31,$F31=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="W31" s="29" t="str">
+        <f>IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(W$5=$E31,$F31=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="X31" s="29" t="str">
+        <f>IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(X$5=$E31,$F31=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="Y31" s="29" t="str">
+        <f>IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(Y$5=$E31,$F31=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="Z31" s="29" t="str">
+        <f>IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(Z$5=$E31,$F31=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="AA31" s="29" t="str">
+        <f>IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AA$5=$E31,$F31=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="AB31" s="29" t="str">
+        <f>IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AB$5=$E31,$F31=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="AC31" s="29" t="str">
+        <f>IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AC$5=$E31,$F31=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="AD31" s="29" t="str">
+        <f>IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AD$5=$E31,$F31=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="AE31" s="29" t="str">
+        <f>IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AE$5=$E31,$F31=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="AF31" s="29" t="str">
+        <f>IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AF$5=$E31,$F31=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="AG31" s="29" t="str">
+        <f>IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AG$5=$E31,$F31=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="AH31" s="29" t="str">
+        <f>IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AH$5=$E31,$F31=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="AI31" s="29" t="str">
+        <f>IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AI$5=$E31,$F31=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="AJ31" s="29" t="str">
+        <f>IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AJ$5=$E31,$F31=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="AK31" s="29" t="str">
+        <f>IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AK$5=$E31,$F31=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="AL31" s="29" t="str">
+        <f>IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AL$5=$E31,$F31=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="AM31" s="29" t="str">
+        <f>IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AM$5=$E31,$F31=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="AN31" s="29" t="str">
+        <f>IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AN$5=$E31,$F31=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="AO31" s="29" t="str">
+        <f>IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AO$5=$E31,$F31=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="AP31" s="29" t="str">
+        <f>IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AP$5=$E31,$F31=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="AQ31" s="29" t="str">
+        <f>IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AQ$5=$E31,$F31=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="AR31" s="29" t="str">
+        <f>IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AR$5=$E31,$F31=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="AS31" s="29" t="str">
+        <f>IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AS$5=$E31,$F31=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="AT31" s="29" t="str">
+        <f>IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AT$5=$E31,$F31=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="AU31" s="29" t="str">
+        <f>IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AU$5=$E31,$F31=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="AV31" s="29" t="str">
+        <f>IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AV$5=$E31,$F31=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="AW31" s="29" t="str">
+        <f>IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AW$5=$E31,$F31=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="AX31" s="29" t="str">
+        <f>IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AX$5=$E31,$F31=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="AY31" s="29" t="str">
+        <f>IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AY$5=$E31,$F31=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="AZ31" s="29" t="str">
+        <f>IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AZ$5=$E31,$F31=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="BA31" s="29" t="str">
+        <f>IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(BA$5=$E31,$F31=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="BB31" s="29" t="str">
+        <f>IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(BB$5=$E31,$F31=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="BC31" s="29" t="str">
+        <f>IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(BC$5=$E31,$F31=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="BD31" s="29" t="str">
+        <f>IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(BD$5=$E31,$F31=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="BE31" s="29" t="str">
+        <f>IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(BE$5=$E31,$F31=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="BF31" s="29" t="str">
+        <f>IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(BF$5=$E31,$F31=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="BG31" s="29" t="str">
+        <f>IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(BG$5=$E31,$F31=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="BH31" s="29" t="str">
+        <f>IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(BH$5=$E31,$F31=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="BI31" s="29" t="str">
+        <f>IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(BI$5=$E31,$F31=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="BJ31" s="29" t="str">
+        <f>IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(BJ$5=$E31,$F31=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="BK31" s="29" t="str">
+        <f>IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(BK$5=$E31,$F31=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="32" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A32" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="B31" s="19" t="s">
-        <v>15</v>
-      </c>
-      <c r="C31" s="19"/>
-      <c r="D31" s="19"/>
-      <c r="E31" s="32"/>
-      <c r="F31" s="19"/>
-      <c r="G31" s="30"/>
-      <c r="H31" s="28"/>
-      <c r="I31" s="28"/>
-      <c r="J31" s="28"/>
-      <c r="K31" s="28"/>
-      <c r="L31" s="28"/>
-      <c r="M31" s="28"/>
-      <c r="N31" s="28"/>
-      <c r="O31" s="28"/>
-      <c r="P31" s="28"/>
-      <c r="Q31" s="28"/>
-      <c r="R31" s="28"/>
-      <c r="S31" s="28"/>
-      <c r="T31" s="28"/>
-      <c r="U31" s="28"/>
-      <c r="V31" s="28"/>
-      <c r="W31" s="28"/>
-      <c r="X31" s="28"/>
-      <c r="Y31" s="28"/>
-      <c r="Z31" s="28"/>
-      <c r="AA31" s="28"/>
-      <c r="AB31" s="28"/>
-      <c r="AC31" s="28"/>
-      <c r="AD31" s="28"/>
-      <c r="AE31" s="28"/>
-      <c r="AF31" s="28"/>
-      <c r="AG31" s="28"/>
-      <c r="AH31" s="28"/>
-      <c r="AI31" s="28"/>
-      <c r="AJ31" s="28"/>
-      <c r="AK31" s="28"/>
-      <c r="AL31" s="28"/>
-      <c r="AM31" s="28"/>
-      <c r="AN31" s="28"/>
-      <c r="AO31" s="28"/>
-      <c r="AP31" s="28"/>
-      <c r="AQ31" s="28"/>
-      <c r="AR31" s="28"/>
-      <c r="AS31" s="28"/>
-      <c r="AT31" s="28"/>
-      <c r="AU31" s="28"/>
-      <c r="AV31" s="28"/>
-      <c r="AW31" s="28"/>
-      <c r="AX31" s="28"/>
-      <c r="AY31" s="28"/>
-      <c r="AZ31" s="28"/>
-      <c r="BA31" s="28"/>
-      <c r="BB31" s="28"/>
-      <c r="BC31" s="28"/>
-      <c r="BD31" s="28"/>
-      <c r="BE31" s="28"/>
-      <c r="BF31" s="28"/>
-      <c r="BG31" s="28"/>
-      <c r="BH31" s="28"/>
-      <c r="BI31" s="28"/>
-      <c r="BJ31" s="28"/>
-      <c r="BK31" s="28"/>
+      <c r="B32" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="C32" s="19"/>
+      <c r="D32" s="19"/>
+      <c r="E32" s="32"/>
+      <c r="F32" s="19"/>
+      <c r="G32" s="30"/>
+      <c r="H32" s="28"/>
+      <c r="I32" s="28"/>
+      <c r="J32" s="28"/>
+      <c r="K32" s="28"/>
+      <c r="L32" s="28"/>
+      <c r="M32" s="28"/>
+      <c r="N32" s="28"/>
+      <c r="O32" s="28"/>
+      <c r="P32" s="28"/>
+      <c r="Q32" s="28"/>
+      <c r="R32" s="28"/>
+      <c r="S32" s="28"/>
+      <c r="T32" s="28"/>
+      <c r="U32" s="28"/>
+      <c r="V32" s="28"/>
+      <c r="W32" s="28"/>
+      <c r="X32" s="28"/>
+      <c r="Y32" s="28"/>
+      <c r="Z32" s="28"/>
+      <c r="AA32" s="28"/>
+      <c r="AB32" s="28"/>
+      <c r="AC32" s="28"/>
+      <c r="AD32" s="28"/>
+      <c r="AE32" s="28"/>
+      <c r="AF32" s="28"/>
+      <c r="AG32" s="28"/>
+      <c r="AH32" s="28"/>
+      <c r="AI32" s="28"/>
+      <c r="AJ32" s="28"/>
+      <c r="AK32" s="28"/>
+      <c r="AL32" s="28"/>
+      <c r="AM32" s="28"/>
+      <c r="AN32" s="28"/>
+      <c r="AO32" s="28"/>
+      <c r="AP32" s="28"/>
+      <c r="AQ32" s="28"/>
+      <c r="AR32" s="28"/>
+      <c r="AS32" s="28"/>
+      <c r="AT32" s="28"/>
+      <c r="AU32" s="28"/>
+      <c r="AV32" s="28"/>
+      <c r="AW32" s="28"/>
+      <c r="AX32" s="28"/>
+      <c r="AY32" s="28"/>
+      <c r="AZ32" s="28"/>
+      <c r="BA32" s="28"/>
+      <c r="BB32" s="28"/>
+      <c r="BC32" s="28"/>
+      <c r="BD32" s="28"/>
+      <c r="BE32" s="28"/>
+      <c r="BF32" s="28"/>
+      <c r="BG32" s="28"/>
+      <c r="BH32" s="28"/>
+      <c r="BI32" s="28"/>
+      <c r="BJ32" s="28"/>
+      <c r="BK32" s="28"/>
     </row>
-    <row r="32" spans="1:63" ht="30" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="C32" s="5"/>
-      <c r="F32" s="14"/>
-      <c r="G32" s="4"/>
+    <row r="33" spans="3:7" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="C33" s="5"/>
+      <c r="F33" s="14"/>
+      <c r="G33" s="4"/>
     </row>
-    <row r="33" spans="3:3" ht="30" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="C33" s="6"/>
+    <row r="34" spans="3:7" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="C34" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -7480,8 +6897,8 @@
     <mergeCell ref="E2:F2"/>
     <mergeCell ref="C4:D4"/>
   </mergeCells>
-  <conditionalFormatting sqref="D6:D30">
-    <cfRule type="dataBar" priority="10">
+  <conditionalFormatting sqref="D19:D31 D12 D6:D8">
+    <cfRule type="dataBar" priority="15">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -7494,19 +6911,61 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H8:BK30">
-    <cfRule type="expression" dxfId="2" priority="78">
+  <conditionalFormatting sqref="H8:BK31">
+    <cfRule type="expression" dxfId="2" priority="83">
       <formula>H$5&lt;=Heute</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H7:BK30">
-    <cfRule type="expression" dxfId="1" priority="11" stopIfTrue="1">
+  <conditionalFormatting sqref="H7:BK31">
+    <cfRule type="expression" dxfId="1" priority="16" stopIfTrue="1">
       <formula>AND(H$5&gt;=$E7+1,H$5&lt;=$E7+$F7-2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H5:BK6">
-    <cfRule type="expression" dxfId="0" priority="1">
+    <cfRule type="expression" dxfId="0" priority="6">
       <formula>H$5&lt;=TODAY()</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D11">
+    <cfRule type="dataBar" priority="4">
+      <dataBar>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color theme="0" tint="-0.14999847407452621"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{D21556E8-F672-4265-9153-D98C5D87D31C}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D13:D18">
+    <cfRule type="dataBar" priority="2">
+      <dataBar>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color theme="0" tint="-0.14999847407452621"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{2F652D15-6590-4BC9-A1FB-CB3096BFA514}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D9:D10">
+    <cfRule type="dataBar" priority="1">
+      <dataBar>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color theme="0" tint="-0.14999847407452621"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{4384F648-93C6-4D30-BBEF-B2C34824E580}</x14:id>
+        </ext>
+      </extLst>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
@@ -7569,10 +7028,10 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>D6:D30</xm:sqref>
+          <xm:sqref>D19:D31 D12 D6:D8</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="2" id="{6C427F2E-2EF5-46B4-BFA6-7C68148277AC}">
+          <x14:cfRule type="iconSet" priority="7" id="{6C427F2E-2EF5-46B4-BFA6-7C68148277AC}">
             <x14:iconSet iconSet="3Flags" showValue="0" custom="1">
               <x14:cfvo type="percent">
                 <xm:f>0</xm:f>
@@ -7591,7 +7050,52 @@
           <xm:sqref>F4</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="85" id="{628A03C6-EE71-4B44-A6BA-69DC45906EA6}">
+          <x14:cfRule type="dataBar" id="{D21556E8-F672-4265-9153-D98C5D87D31C}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="num">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>D11</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{2F652D15-6590-4BC9-A1FB-CB3096BFA514}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="num">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>D13:D18</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{4384F648-93C6-4D30-BBEF-B2C34824E580}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="num">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>D9:D10</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="iconSet" priority="125" id="{628A03C6-EE71-4B44-A6BA-69DC45906EA6}">
             <x14:iconSet iconSet="3Stars" showValue="0" custom="1">
               <x14:cfvo type="percent">
                 <xm:f>0</xm:f>
@@ -7607,7 +7111,7 @@
               <x14:cfIcon iconSet="3Signs" iconId="0"/>
             </x14:iconSet>
           </x14:cfRule>
-          <xm:sqref>H7:BK30</xm:sqref>
+          <xm:sqref>H7:BK31</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
@@ -7621,7 +7125,7 @@
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.06640625" defaultRowHeight="12.9" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.06640625" defaultRowHeight="13.3" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="87.06640625" style="10" customWidth="1"/>
     <col min="2" max="16384" width="9.06640625" style="8"/>
@@ -7629,22 +7133,22 @@
   <sheetData>
     <row r="1" spans="1:1" s="9" customFormat="1" ht="50.15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A1" s="33" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="150" x14ac:dyDescent="0.45">
       <c r="A2" s="34" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="26.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A3" s="33" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:1" s="10" customFormat="1" ht="222" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A4" s="11" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated Zeitplan: added phase 4
</commit_message>
<xml_diff>
--- a/docs/Zeitplan.xlsx
+++ b/docs/Zeitplan.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E4BA6EF-4B11-4112-A519-979C3A766F6D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{278EFC7B-4B87-4C2C-8401-D26EA28BCAD9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="11949" tabRatio="415" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="52">
   <si>
     <t>Erstellen Sie auf diesem Arbeitsblatt ein Gantt-Diagramm.
 Geben Sie den Titel dieses Projekts in Zelle B1 ein. 
@@ -81,9 +81,6 @@
   <si>
     <t>Diese Zeile markiert das Ende der Gantt-Meilensteindaten. Geben Sie in dieser Zeile NICHTS EIN. 
 Um weitere Elemente hinzuzufügen, fügen Sie neue Zeilen über dieser ein.</t>
-  </si>
-  <si>
-    <t>Meilensteinbeschreibung</t>
   </si>
   <si>
     <t>Um weitere Daten hinzuzufügen, fügen Sie neue Zeilen ÜBER dieser ein.</t>
@@ -134,9 +131,6 @@
 Geben Sie das Projektanfangsdatum in Zelle E2 ein, oder erlauben Sie es der Beispielformel, den kleinsten Datumswert in der Gantt-Datentabelle zu suchen. Projektanfangsdatum: Die Bezeichnung steht in Zelle C2.</t>
   </si>
   <si>
-    <t>GPIO-Simulator</t>
-  </si>
-  <si>
     <t>Projektvereinbarung</t>
   </si>
   <si>
@@ -185,9 +179,6 @@
     <t>User Guide schreiben</t>
   </si>
   <si>
-    <t>Beispiel-Projekt implementieren</t>
-  </si>
-  <si>
     <t>Generelle Aufbaumöglichkeiten definieren</t>
   </si>
   <si>
@@ -207,6 +198,27 @@
   </si>
   <si>
     <t>Meileistein: Projekt fertigstellen</t>
+  </si>
+  <si>
+    <t>Beispielprojekt implementieren</t>
+  </si>
+  <si>
+    <t>Beschreibung des Tasks</t>
+  </si>
+  <si>
+    <t>Meilenstein: IP5 beenden</t>
+  </si>
+  <si>
+    <t>Phase 4: Abgabe und Fertigstellung IP5</t>
+  </si>
+  <si>
+    <t>Präsentation: Vorbereitung und Durchführung</t>
+  </si>
+  <si>
+    <t>Projektabgabe: Hardware und Source Code</t>
+  </si>
+  <si>
+    <t>IP5: GPIO-Simulator</t>
   </si>
 </sst>
 </file>
@@ -1159,6 +1171,24 @@
     <xf numFmtId="168" fontId="25" fillId="37" borderId="0" xfId="10" applyFont="1" applyFill="1" applyBorder="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="28" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="28" fillId="0" borderId="0" xfId="9" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="28" fillId="0" borderId="0" xfId="10" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="8" applyFont="1">
       <alignment horizontal="right" vertical="center" indent="1"/>
     </xf>
@@ -1176,24 +1206,6 @@
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="2" xfId="8" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="28" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="28" fillId="0" borderId="0" xfId="9" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="168" fontId="28" fillId="0" borderId="0" xfId="10" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="50">
@@ -1248,7 +1260,151 @@
     <cellStyle name="Zelle überprüfen" xfId="22" builtinId="23" customBuiltin="1"/>
     <cellStyle name="zHiddenText" xfId="3" xr:uid="{00000000-0005-0000-0000-000031000000}"/>
   </cellStyles>
-  <dxfs count="23">
+  <dxfs count="31">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="8" tint="-0.499984740745262"/>
+        </left>
+        <right style="thin">
+          <color theme="8" tint="-0.499984740745262"/>
+        </right>
+        <top style="thin">
+          <color theme="0"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="8" tint="-0.499984740745262"/>
+        </left>
+        <right style="thin">
+          <color theme="8" tint="-0.499984740745262"/>
+        </right>
+        <top style="thin">
+          <color theme="0"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="8" tint="-0.499984740745262"/>
+        </left>
+        <right style="thin">
+          <color theme="8" tint="-0.499984740745262"/>
+        </right>
+        <top style="thin">
+          <color theme="0"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="8" tint="-0.499984740745262"/>
+        </left>
+        <right style="thin">
+          <color theme="8" tint="-0.499984740745262"/>
+        </right>
+        <top style="thin">
+          <color theme="0"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1587,20 +1743,20 @@
   </dxfs>
   <tableStyles count="2" defaultTableStyle="Gantt Table Style" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="Gantt Table Style" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
-      <tableStyleElement type="wholeTable" dxfId="22"/>
-      <tableStyleElement type="headerRow" dxfId="21"/>
-      <tableStyleElement type="firstRowStripe" dxfId="20"/>
+      <tableStyleElement type="wholeTable" dxfId="30"/>
+      <tableStyleElement type="headerRow" dxfId="29"/>
+      <tableStyleElement type="firstRowStripe" dxfId="28"/>
     </tableStyle>
     <tableStyle name="ToDoList" pivot="0" count="9" xr9:uid="{00000000-0011-0000-FFFF-FFFF01000000}">
-      <tableStyleElement type="wholeTable" dxfId="19"/>
-      <tableStyleElement type="headerRow" dxfId="18"/>
-      <tableStyleElement type="totalRow" dxfId="17"/>
-      <tableStyleElement type="firstColumn" dxfId="16"/>
-      <tableStyleElement type="lastColumn" dxfId="15"/>
-      <tableStyleElement type="firstRowStripe" dxfId="14"/>
-      <tableStyleElement type="secondRowStripe" dxfId="13"/>
-      <tableStyleElement type="firstColumnStripe" dxfId="12"/>
-      <tableStyleElement type="secondColumnStripe" dxfId="11"/>
+      <tableStyleElement type="wholeTable" dxfId="27"/>
+      <tableStyleElement type="headerRow" dxfId="26"/>
+      <tableStyleElement type="totalRow" dxfId="25"/>
+      <tableStyleElement type="firstColumn" dxfId="24"/>
+      <tableStyleElement type="lastColumn" dxfId="23"/>
+      <tableStyleElement type="firstRowStripe" dxfId="22"/>
+      <tableStyleElement type="secondRowStripe" dxfId="21"/>
+      <tableStyleElement type="firstColumnStripe" dxfId="20"/>
+      <tableStyleElement type="secondColumnStripe" dxfId="19"/>
     </tableStyle>
   </tableStyles>
   <colors>
@@ -1742,8 +1898,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Meilensteine" displayName="Meilensteine" ref="B6:F32" totalsRowShown="0">
-  <autoFilter ref="B6:F32" xr:uid="{00000000-0009-0000-0100-000001000000}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Meilensteine" displayName="Meilensteine" ref="B6:F35" totalsRowShown="0">
+  <autoFilter ref="B6:F35" xr:uid="{00000000-0009-0000-0100-000001000000}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -1751,7 +1907,7 @@
     <filterColumn colId="4" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Meilensteinbeschreibung"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Beschreibung des Tasks"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Zugewiesen an"/>
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Fortschritt"/>
     <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Start"/>
@@ -2029,10 +2185,10 @@
   <sheetPr codeName="Sheet1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:BK35"/>
+  <dimension ref="A1:BK38"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="A10" zoomScale="69" zoomScaleNormal="50" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="S18" sqref="S18"/>
+    <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScale="58" zoomScaleNormal="50" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="P14" sqref="P14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.06640625" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.45"/>
@@ -2052,7 +2208,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="15" t="s">
-        <v>23</v>
+        <v>51</v>
       </c>
       <c r="C1" s="1"/>
       <c r="E1"/>
@@ -2062,18 +2218,18 @@
     </row>
     <row r="2" spans="1:63" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A2" s="13" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B2" s="16"/>
-      <c r="C2" s="58" t="s">
-        <v>11</v>
-      </c>
-      <c r="D2" s="59"/>
-      <c r="E2" s="60">
+      <c r="C2" s="64" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="65"/>
+      <c r="E2" s="66">
         <f ca="1">IFERROR(IF(MIN(Meilensteine[Start])=0,TODAY(),MIN(Meilensteine[Start])),TODAY())</f>
         <v>43864</v>
       </c>
-      <c r="F2" s="61"/>
+      <c r="F2" s="67"/>
       <c r="I2" s="36"/>
       <c r="J2" s="36"/>
       <c r="K2" s="36"/>
@@ -2086,10 +2242,10 @@
         <v>1</v>
       </c>
       <c r="B3" s="16"/>
-      <c r="C3" s="58" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" s="59"/>
+      <c r="C3" s="64" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="65"/>
       <c r="E3" s="39">
         <v>53</v>
       </c>
@@ -2104,10 +2260,10 @@
       <c r="A4" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="62" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" s="63"/>
+      <c r="C4" s="68" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="69"/>
       <c r="E4" s="40">
         <v>1</v>
       </c>
@@ -2432,19 +2588,19 @@
         <v>4</v>
       </c>
       <c r="B6" s="22" t="s">
-        <v>9</v>
+        <v>46</v>
       </c>
       <c r="C6" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="D6" s="23" t="s">
+      <c r="E6" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="E6" s="23" t="s">
+      <c r="F6" s="23" t="s">
         <v>16</v>
-      </c>
-      <c r="F6" s="23" t="s">
-        <v>17</v>
       </c>
       <c r="G6" s="21"/>
       <c r="H6" s="42" t="str">
@@ -2743,7 +2899,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="53" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C8" s="54"/>
       <c r="D8" s="55"/>
@@ -2980,7 +3136,7 @@
     <row r="9" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A9" s="12"/>
       <c r="B9" s="31" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C9" s="23"/>
       <c r="D9" s="24">
@@ -3221,7 +3377,7 @@
     <row r="10" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A10" s="12"/>
       <c r="B10" s="31" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C10" s="23"/>
       <c r="D10" s="24">
@@ -3461,15 +3617,17 @@
     </row>
     <row r="11" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A11" s="12"/>
-      <c r="B11" s="64" t="s">
-        <v>44</v>
-      </c>
-      <c r="C11" s="65"/>
-      <c r="D11" s="66"/>
-      <c r="E11" s="67">
+      <c r="B11" s="58" t="s">
+        <v>41</v>
+      </c>
+      <c r="C11" s="59"/>
+      <c r="D11" s="60">
+        <v>1</v>
+      </c>
+      <c r="E11" s="61">
         <v>43881</v>
       </c>
-      <c r="F11" s="68">
+      <c r="F11" s="62">
         <v>1</v>
       </c>
       <c r="G11" s="20"/>
@@ -3533,7 +3691,7 @@
     <row r="12" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A12" s="12"/>
       <c r="B12" s="53" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C12" s="54"/>
       <c r="D12" s="55"/>
@@ -3600,7 +3758,7 @@
     <row r="13" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A13" s="12"/>
       <c r="B13" s="31" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C13" s="23"/>
       <c r="D13" s="24">
@@ -3841,7 +3999,7 @@
     <row r="14" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A14" s="12"/>
       <c r="B14" s="31" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C14" s="23"/>
       <c r="D14" s="24">
@@ -4082,7 +4240,7 @@
     <row r="15" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A15" s="12"/>
       <c r="B15" s="31" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C15" s="23"/>
       <c r="D15" s="24">
@@ -4323,7 +4481,7 @@
     <row r="16" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A16" s="12"/>
       <c r="B16" s="31" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C16" s="23"/>
       <c r="D16" s="24">
@@ -4564,7 +4722,7 @@
     <row r="17" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A17" s="12"/>
       <c r="B17" s="31" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C17" s="23"/>
       <c r="D17" s="24">
@@ -4805,7 +4963,7 @@
     <row r="18" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A18" s="12"/>
       <c r="B18" s="31" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C18" s="23"/>
       <c r="D18" s="24">
@@ -5045,17 +5203,17 @@
     </row>
     <row r="19" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A19" s="12"/>
-      <c r="B19" s="64" t="s">
-        <v>45</v>
-      </c>
-      <c r="C19" s="65"/>
-      <c r="D19" s="66">
+      <c r="B19" s="58" t="s">
+        <v>42</v>
+      </c>
+      <c r="C19" s="59"/>
+      <c r="D19" s="60">
         <v>0</v>
       </c>
-      <c r="E19" s="67">
+      <c r="E19" s="61">
         <v>43957</v>
       </c>
-      <c r="F19" s="68">
+      <c r="F19" s="62">
         <v>1</v>
       </c>
       <c r="G19" s="20"/>
@@ -5287,7 +5445,7 @@
     <row r="20" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A20" s="13"/>
       <c r="B20" s="53" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C20" s="54"/>
       <c r="D20" s="55"/>
@@ -5522,7 +5680,7 @@
     <row r="21" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A21" s="13"/>
       <c r="B21" s="31" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C21" s="27"/>
       <c r="D21" s="24">
@@ -5763,7 +5921,7 @@
     <row r="22" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A22" s="12"/>
       <c r="B22" s="31" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C22" s="27"/>
       <c r="D22" s="24">
@@ -6004,7 +6162,7 @@
     <row r="23" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A23" s="12"/>
       <c r="B23" s="31" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C23" s="27"/>
       <c r="D23" s="24">
@@ -6244,17 +6402,17 @@
     </row>
     <row r="24" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A24" s="12"/>
-      <c r="B24" s="64" t="s">
-        <v>46</v>
-      </c>
-      <c r="C24" s="69"/>
-      <c r="D24" s="66">
+      <c r="B24" s="58" t="s">
+        <v>43</v>
+      </c>
+      <c r="C24" s="63"/>
+      <c r="D24" s="60">
         <v>0</v>
       </c>
-      <c r="E24" s="67">
+      <c r="E24" s="61">
         <v>43985</v>
       </c>
-      <c r="F24" s="68">
+      <c r="F24" s="62">
         <v>1</v>
       </c>
       <c r="G24" s="20"/>
@@ -6486,7 +6644,7 @@
     <row r="25" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A25" s="12"/>
       <c r="B25" s="53" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C25" s="54"/>
       <c r="D25" s="55"/>
@@ -6721,7 +6879,7 @@
     <row r="26" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A26" s="12"/>
       <c r="B26" s="31" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C26" s="27"/>
       <c r="D26" s="24">
@@ -6962,7 +7120,7 @@
     <row r="27" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A27" s="12"/>
       <c r="B27" s="31" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C27" s="27"/>
       <c r="D27" s="24">
@@ -7203,7 +7361,7 @@
     <row r="28" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A28" s="12"/>
       <c r="B28" s="31" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C28" s="27"/>
       <c r="D28" s="24">
@@ -7444,7 +7602,7 @@
     <row r="29" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A29" s="12"/>
       <c r="B29" s="31" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C29" s="27"/>
       <c r="D29" s="24">
@@ -7685,89 +7843,257 @@
     <row r="30" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A30" s="12"/>
       <c r="B30" s="31" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="C30" s="27"/>
       <c r="D30" s="24">
         <v>0</v>
       </c>
       <c r="E30" s="52">
-        <v>44020</v>
+        <v>44027</v>
       </c>
       <c r="F30" s="26">
         <v>0</v>
       </c>
       <c r="G30" s="20"/>
-      <c r="H30" s="29"/>
-      <c r="I30" s="29"/>
-      <c r="J30" s="29"/>
-      <c r="K30" s="29"/>
-      <c r="L30" s="29"/>
-      <c r="M30" s="29"/>
-      <c r="N30" s="29"/>
-      <c r="O30" s="29"/>
-      <c r="P30" s="29"/>
-      <c r="Q30" s="29"/>
-      <c r="R30" s="29"/>
-      <c r="S30" s="29"/>
-      <c r="T30" s="29"/>
-      <c r="U30" s="29"/>
-      <c r="V30" s="29"/>
-      <c r="W30" s="29"/>
-      <c r="X30" s="29"/>
-      <c r="Y30" s="29"/>
-      <c r="Z30" s="29"/>
-      <c r="AA30" s="29"/>
-      <c r="AB30" s="29"/>
-      <c r="AC30" s="29"/>
-      <c r="AD30" s="29"/>
-      <c r="AE30" s="29"/>
-      <c r="AF30" s="29"/>
-      <c r="AG30" s="29"/>
-      <c r="AH30" s="29"/>
-      <c r="AI30" s="29"/>
-      <c r="AJ30" s="29"/>
-      <c r="AK30" s="29"/>
-      <c r="AL30" s="29"/>
-      <c r="AM30" s="29"/>
-      <c r="AN30" s="29"/>
-      <c r="AO30" s="29"/>
-      <c r="AP30" s="29"/>
-      <c r="AQ30" s="29"/>
-      <c r="AR30" s="29"/>
-      <c r="AS30" s="29"/>
-      <c r="AT30" s="29"/>
-      <c r="AU30" s="29"/>
-      <c r="AV30" s="29"/>
-      <c r="AW30" s="29"/>
-      <c r="AX30" s="29"/>
-      <c r="AY30" s="29"/>
-      <c r="AZ30" s="29"/>
-      <c r="BA30" s="29"/>
-      <c r="BB30" s="29"/>
-      <c r="BC30" s="29"/>
-      <c r="BD30" s="29"/>
-      <c r="BE30" s="29"/>
-      <c r="BF30" s="29"/>
-      <c r="BG30" s="29"/>
-      <c r="BH30" s="29"/>
-      <c r="BI30" s="29"/>
-      <c r="BJ30" s="29"/>
-      <c r="BK30" s="29"/>
+      <c r="H30" s="29" t="str">
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(H$5=$E30,$F30=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="I30" s="29" t="str">
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(I$5=$E30,$F30=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="J30" s="29" t="str">
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(J$5=$E30,$F30=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="K30" s="29" t="str">
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(K$5=$E30,$F30=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="L30" s="29" t="str">
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(L$5=$E30,$F30=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="M30" s="29" t="str">
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(M$5=$E30,$F30=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="N30" s="29" t="str">
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(N$5=$E30,$F30=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="O30" s="29" t="str">
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(O$5=$E30,$F30=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="P30" s="29" t="str">
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(P$5=$E30,$F30=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="Q30" s="29" t="str">
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(Q$5=$E30,$F30=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="R30" s="29" t="str">
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(R$5=$E30,$F30=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="S30" s="29" t="str">
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(S$5=$E30,$F30=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="T30" s="29" t="str">
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(T$5=$E30,$F30=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="U30" s="29" t="str">
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(U$5=$E30,$F30=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="V30" s="29" t="str">
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(V$5=$E30,$F30=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="W30" s="29" t="str">
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(W$5=$E30,$F30=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="X30" s="29" t="str">
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(X$5=$E30,$F30=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="Y30" s="29" t="str">
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(Y$5=$E30,$F30=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="Z30" s="29" t="str">
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(Z$5=$E30,$F30=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="AA30" s="29" t="str">
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AA$5=$E30,$F30=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="AB30" s="29" t="str">
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AB$5=$E30,$F30=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="AC30" s="29" t="str">
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AC$5=$E30,$F30=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="AD30" s="29" t="str">
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AD$5=$E30,$F30=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="AE30" s="29" t="str">
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AE$5=$E30,$F30=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="AF30" s="29" t="str">
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AF$5=$E30,$F30=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="AG30" s="29" t="str">
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AG$5=$E30,$F30=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="AH30" s="29" t="str">
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AH$5=$E30,$F30=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="AI30" s="29" t="str">
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AI$5=$E30,$F30=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="AJ30" s="29" t="str">
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AJ$5=$E30,$F30=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="AK30" s="29" t="str">
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AK$5=$E30,$F30=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="AL30" s="29" t="str">
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AL$5=$E30,$F30=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="AM30" s="29" t="str">
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AM$5=$E30,$F30=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="AN30" s="29" t="str">
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AN$5=$E30,$F30=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="AO30" s="29" t="str">
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AO$5=$E30,$F30=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="AP30" s="29" t="str">
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AP$5=$E30,$F30=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="AQ30" s="29" t="str">
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AQ$5=$E30,$F30=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="AR30" s="29" t="str">
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AR$5=$E30,$F30=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="AS30" s="29" t="str">
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AS$5=$E30,$F30=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="AT30" s="29" t="str">
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AT$5=$E30,$F30=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="AU30" s="29" t="str">
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AU$5=$E30,$F30=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="AV30" s="29" t="str">
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AV$5=$E30,$F30=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="AW30" s="29" t="str">
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AW$5=$E30,$F30=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="AX30" s="29" t="str">
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AX$5=$E30,$F30=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="AY30" s="29" t="str">
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AY$5=$E30,$F30=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="AZ30" s="29" t="str">
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AZ$5=$E30,$F30=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="BA30" s="29" t="str">
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(BA$5=$E30,$F30=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="BB30" s="29" t="str">
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(BB$5=$E30,$F30=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="BC30" s="29" t="str">
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(BC$5=$E30,$F30=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="BD30" s="29" t="str">
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(BD$5=$E30,$F30=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="BE30" s="29" t="str">
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(BE$5=$E30,$F30=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="BF30" s="29" t="str">
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(BF$5=$E30,$F30=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="BG30" s="29" t="str">
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(BG$5=$E30,$F30=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="BH30" s="29" t="str">
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(BH$5=$E30,$F30=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="BI30" s="29" t="str">
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(BI$5=$E30,$F30=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="BJ30" s="29" t="str">
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(BJ$5=$E30,$F30=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="BK30" s="29" t="str">
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(BK$5=$E30,$F30=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
     </row>
     <row r="31" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A31" s="12"/>
-      <c r="B31" s="64" t="s">
-        <v>47</v>
-      </c>
-      <c r="C31" s="69"/>
-      <c r="D31" s="66">
+      <c r="B31" s="58" t="s">
+        <v>44</v>
+      </c>
+      <c r="C31" s="63"/>
+      <c r="D31" s="60">
         <v>0</v>
       </c>
-      <c r="E31" s="67">
+      <c r="E31" s="61">
         <v>44048</v>
       </c>
-      <c r="F31" s="68">
+      <c r="F31" s="62">
         <v>1</v>
       </c>
       <c r="G31" s="20"/>
@@ -7997,14 +8323,14 @@
       </c>
     </row>
     <row r="32" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A32" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="B32" s="31"/>
-      <c r="C32" s="27"/>
-      <c r="D32" s="24"/>
-      <c r="E32" s="52"/>
-      <c r="F32" s="26"/>
+      <c r="A32" s="12"/>
+      <c r="B32" s="53" t="s">
+        <v>48</v>
+      </c>
+      <c r="C32" s="54"/>
+      <c r="D32" s="55"/>
+      <c r="E32" s="56"/>
+      <c r="F32" s="57"/>
       <c r="G32" s="20"/>
       <c r="H32" s="29" t="str">
         <f>IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(H$5=$E32,$F32=1),Meilenstein_Markierung,"")),"")</f>
@@ -8231,82 +8557,811 @@
         <v/>
       </c>
     </row>
-    <row r="33" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A33" s="13" t="s">
+    <row r="33" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A33" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="B33" s="31" t="s">
+        <v>49</v>
+      </c>
+      <c r="C33" s="27"/>
+      <c r="D33" s="24">
+        <v>0</v>
+      </c>
+      <c r="E33" s="52">
+        <v>44084</v>
+      </c>
+      <c r="F33" s="26">
+        <v>0</v>
+      </c>
+      <c r="G33" s="20"/>
+      <c r="H33" s="29" t="str">
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(H$5=$E33,$F33=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="I33" s="29" t="str">
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(I$5=$E33,$F33=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="J33" s="29" t="str">
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(J$5=$E33,$F33=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="K33" s="29" t="str">
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(K$5=$E33,$F33=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="L33" s="29" t="str">
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(L$5=$E33,$F33=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="M33" s="29" t="str">
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(M$5=$E33,$F33=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="N33" s="29" t="str">
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(N$5=$E33,$F33=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="O33" s="29" t="str">
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(O$5=$E33,$F33=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="P33" s="29" t="str">
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(P$5=$E33,$F33=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="Q33" s="29" t="str">
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(Q$5=$E33,$F33=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="R33" s="29" t="str">
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(R$5=$E33,$F33=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="S33" s="29" t="str">
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(S$5=$E33,$F33=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="T33" s="29" t="str">
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(T$5=$E33,$F33=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="U33" s="29" t="str">
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(U$5=$E33,$F33=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="V33" s="29" t="str">
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(V$5=$E33,$F33=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="W33" s="29" t="str">
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(W$5=$E33,$F33=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="X33" s="29" t="str">
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(X$5=$E33,$F33=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="Y33" s="29" t="str">
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(Y$5=$E33,$F33=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="Z33" s="29" t="str">
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(Z$5=$E33,$F33=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="AA33" s="29" t="str">
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AA$5=$E33,$F33=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="AB33" s="29" t="str">
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AB$5=$E33,$F33=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="AC33" s="29" t="str">
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AC$5=$E33,$F33=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="AD33" s="29" t="str">
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AD$5=$E33,$F33=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="AE33" s="29" t="str">
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AE$5=$E33,$F33=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="AF33" s="29" t="str">
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AF$5=$E33,$F33=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="AG33" s="29" t="str">
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AG$5=$E33,$F33=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="AH33" s="29" t="str">
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AH$5=$E33,$F33=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="AI33" s="29" t="str">
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AI$5=$E33,$F33=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="AJ33" s="29" t="str">
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AJ$5=$E33,$F33=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="AK33" s="29" t="str">
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AK$5=$E33,$F33=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="AL33" s="29" t="str">
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AL$5=$E33,$F33=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="AM33" s="29" t="str">
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AM$5=$E33,$F33=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="AN33" s="29" t="str">
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AN$5=$E33,$F33=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="AO33" s="29" t="str">
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AO$5=$E33,$F33=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="AP33" s="29" t="str">
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AP$5=$E33,$F33=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="AQ33" s="29" t="str">
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AQ$5=$E33,$F33=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="AR33" s="29" t="str">
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AR$5=$E33,$F33=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="AS33" s="29" t="str">
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AS$5=$E33,$F33=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="AT33" s="29" t="str">
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AT$5=$E33,$F33=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="AU33" s="29" t="str">
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AU$5=$E33,$F33=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="AV33" s="29" t="str">
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AV$5=$E33,$F33=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="AW33" s="29" t="str">
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AW$5=$E33,$F33=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="AX33" s="29" t="str">
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AX$5=$E33,$F33=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="AY33" s="29" t="str">
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AY$5=$E33,$F33=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="AZ33" s="29" t="str">
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AZ$5=$E33,$F33=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="BA33" s="29" t="str">
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(BA$5=$E33,$F33=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="BB33" s="29" t="str">
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(BB$5=$E33,$F33=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="BC33" s="29" t="str">
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(BC$5=$E33,$F33=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="BD33" s="29" t="str">
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(BD$5=$E33,$F33=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="BE33" s="29" t="str">
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(BE$5=$E33,$F33=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="BF33" s="29" t="str">
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(BF$5=$E33,$F33=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="BG33" s="29" t="str">
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(BG$5=$E33,$F33=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="BH33" s="29" t="str">
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(BH$5=$E33,$F33=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="BI33" s="29" t="str">
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(BI$5=$E33,$F33=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="BJ33" s="29" t="str">
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(BJ$5=$E33,$F33=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="BK33" s="29" t="str">
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(BK$5=$E33,$F33=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="34" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A34" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="B34" s="31" t="s">
+        <v>50</v>
+      </c>
+      <c r="C34" s="27"/>
+      <c r="D34" s="24">
+        <v>0</v>
+      </c>
+      <c r="E34" s="52">
+        <v>44084</v>
+      </c>
+      <c r="F34" s="26">
+        <v>0</v>
+      </c>
+      <c r="G34" s="20"/>
+      <c r="H34" s="29" t="str">
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(H$5=$E34,$F34=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="I34" s="29" t="str">
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(I$5=$E34,$F34=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="J34" s="29" t="str">
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(J$5=$E34,$F34=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="K34" s="29" t="str">
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(K$5=$E34,$F34=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="L34" s="29" t="str">
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(L$5=$E34,$F34=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="M34" s="29" t="str">
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(M$5=$E34,$F34=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="N34" s="29" t="str">
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(N$5=$E34,$F34=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="O34" s="29" t="str">
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(O$5=$E34,$F34=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="P34" s="29" t="str">
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(P$5=$E34,$F34=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="Q34" s="29" t="str">
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(Q$5=$E34,$F34=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="R34" s="29" t="str">
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(R$5=$E34,$F34=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="S34" s="29" t="str">
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(S$5=$E34,$F34=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="T34" s="29" t="str">
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(T$5=$E34,$F34=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="U34" s="29" t="str">
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(U$5=$E34,$F34=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="V34" s="29" t="str">
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(V$5=$E34,$F34=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="W34" s="29" t="str">
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(W$5=$E34,$F34=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="X34" s="29" t="str">
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(X$5=$E34,$F34=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="Y34" s="29" t="str">
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(Y$5=$E34,$F34=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="Z34" s="29" t="str">
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(Z$5=$E34,$F34=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="AA34" s="29" t="str">
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AA$5=$E34,$F34=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="AB34" s="29" t="str">
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AB$5=$E34,$F34=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="AC34" s="29" t="str">
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AC$5=$E34,$F34=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="AD34" s="29" t="str">
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AD$5=$E34,$F34=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="AE34" s="29" t="str">
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AE$5=$E34,$F34=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="AF34" s="29" t="str">
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AF$5=$E34,$F34=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="AG34" s="29" t="str">
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AG$5=$E34,$F34=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="AH34" s="29" t="str">
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AH$5=$E34,$F34=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="AI34" s="29" t="str">
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AI$5=$E34,$F34=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="AJ34" s="29" t="str">
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AJ$5=$E34,$F34=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="AK34" s="29" t="str">
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AK$5=$E34,$F34=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="AL34" s="29" t="str">
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AL$5=$E34,$F34=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="AM34" s="29" t="str">
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AM$5=$E34,$F34=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="AN34" s="29" t="str">
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AN$5=$E34,$F34=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="AO34" s="29" t="str">
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AO$5=$E34,$F34=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="AP34" s="29" t="str">
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AP$5=$E34,$F34=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="AQ34" s="29" t="str">
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AQ$5=$E34,$F34=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="AR34" s="29" t="str">
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AR$5=$E34,$F34=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="AS34" s="29" t="str">
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AS$5=$E34,$F34=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="AT34" s="29" t="str">
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AT$5=$E34,$F34=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="AU34" s="29" t="str">
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AU$5=$E34,$F34=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="AV34" s="29" t="str">
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AV$5=$E34,$F34=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="AW34" s="29" t="str">
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AW$5=$E34,$F34=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="AX34" s="29" t="str">
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AX$5=$E34,$F34=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="AY34" s="29" t="str">
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AY$5=$E34,$F34=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="AZ34" s="29" t="str">
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AZ$5=$E34,$F34=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="BA34" s="29" t="str">
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(BA$5=$E34,$F34=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="BB34" s="29" t="str">
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(BB$5=$E34,$F34=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="BC34" s="29" t="str">
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(BC$5=$E34,$F34=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="BD34" s="29" t="str">
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(BD$5=$E34,$F34=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="BE34" s="29" t="str">
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(BE$5=$E34,$F34=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="BF34" s="29" t="str">
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(BF$5=$E34,$F34=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="BG34" s="29" t="str">
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(BG$5=$E34,$F34=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="BH34" s="29" t="str">
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(BH$5=$E34,$F34=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="BI34" s="29" t="str">
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(BI$5=$E34,$F34=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="BJ34" s="29" t="str">
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(BJ$5=$E34,$F34=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="BK34" s="29" t="str">
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(BK$5=$E34,$F34=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="35" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A35" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="B35" s="58" t="s">
+        <v>47</v>
+      </c>
+      <c r="C35" s="63"/>
+      <c r="D35" s="60">
+        <v>0</v>
+      </c>
+      <c r="E35" s="61">
+        <v>44084</v>
+      </c>
+      <c r="F35" s="62">
+        <v>0</v>
+      </c>
+      <c r="G35" s="20"/>
+      <c r="H35" s="29" t="str">
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(H$5=$E35,$F35=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="I35" s="29" t="str">
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(I$5=$E35,$F35=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="J35" s="29" t="str">
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(J$5=$E35,$F35=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="K35" s="29" t="str">
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(K$5=$E35,$F35=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="L35" s="29" t="str">
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(L$5=$E35,$F35=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="M35" s="29" t="str">
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(M$5=$E35,$F35=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="N35" s="29" t="str">
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(N$5=$E35,$F35=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="O35" s="29" t="str">
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(O$5=$E35,$F35=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="P35" s="29" t="str">
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(P$5=$E35,$F35=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="Q35" s="29" t="str">
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(Q$5=$E35,$F35=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="R35" s="29" t="str">
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(R$5=$E35,$F35=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="S35" s="29" t="str">
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(S$5=$E35,$F35=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="T35" s="29" t="str">
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(T$5=$E35,$F35=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="U35" s="29" t="str">
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(U$5=$E35,$F35=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="V35" s="29" t="str">
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(V$5=$E35,$F35=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="W35" s="29" t="str">
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(W$5=$E35,$F35=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="X35" s="29" t="str">
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(X$5=$E35,$F35=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="Y35" s="29" t="str">
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(Y$5=$E35,$F35=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="Z35" s="29" t="str">
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(Z$5=$E35,$F35=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="AA35" s="29" t="str">
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AA$5=$E35,$F35=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="AB35" s="29" t="str">
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AB$5=$E35,$F35=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="AC35" s="29" t="str">
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AC$5=$E35,$F35=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="AD35" s="29" t="str">
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AD$5=$E35,$F35=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="AE35" s="29" t="str">
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AE$5=$E35,$F35=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="AF35" s="29" t="str">
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AF$5=$E35,$F35=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="AG35" s="29" t="str">
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AG$5=$E35,$F35=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="AH35" s="29" t="str">
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AH$5=$E35,$F35=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="AI35" s="29" t="str">
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AI$5=$E35,$F35=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="AJ35" s="29" t="str">
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AJ$5=$E35,$F35=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="AK35" s="29" t="str">
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AK$5=$E35,$F35=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="AL35" s="29" t="str">
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AL$5=$E35,$F35=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="AM35" s="29" t="str">
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AM$5=$E35,$F35=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="AN35" s="29" t="str">
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AN$5=$E35,$F35=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="AO35" s="29" t="str">
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AO$5=$E35,$F35=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="AP35" s="29" t="str">
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AP$5=$E35,$F35=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="AQ35" s="29" t="str">
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AQ$5=$E35,$F35=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="AR35" s="29" t="str">
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AR$5=$E35,$F35=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="AS35" s="29" t="str">
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AS$5=$E35,$F35=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="AT35" s="29" t="str">
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AT$5=$E35,$F35=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="AU35" s="29" t="str">
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AU$5=$E35,$F35=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="AV35" s="29" t="str">
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AV$5=$E35,$F35=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="AW35" s="29" t="str">
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AW$5=$E35,$F35=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="AX35" s="29" t="str">
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AX$5=$E35,$F35=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="AY35" s="29" t="str">
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AY$5=$E35,$F35=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="AZ35" s="29" t="str">
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(AZ$5=$E35,$F35=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="BA35" s="29" t="str">
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(BA$5=$E35,$F35=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="BB35" s="29" t="str">
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(BB$5=$E35,$F35=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="BC35" s="29" t="str">
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(BC$5=$E35,$F35=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="BD35" s="29" t="str">
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(BD$5=$E35,$F35=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="BE35" s="29" t="str">
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(BE$5=$E35,$F35=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="BF35" s="29" t="str">
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(BF$5=$E35,$F35=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="BG35" s="29" t="str">
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(BG$5=$E35,$F35=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="BH35" s="29" t="str">
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(BH$5=$E35,$F35=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="BI35" s="29" t="str">
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(BI$5=$E35,$F35=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="BJ35" s="29" t="str">
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(BJ$5=$E35,$F35=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+      <c r="BK35" s="29" t="str">
+        <f ca="1">IFERROR(IF(LEN(Meilensteine[[#This Row],[Anzahl Tage]])=0,"",IF(AND(BK$5=$E35,$F35=1),Meilenstein_Markierung,"")),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="36" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A36" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="B33" s="19" t="s">
-        <v>10</v>
-      </c>
-      <c r="C33" s="19"/>
-      <c r="D33" s="19"/>
-      <c r="E33" s="32"/>
-      <c r="F33" s="19"/>
-      <c r="G33" s="30"/>
-      <c r="H33" s="28"/>
-      <c r="I33" s="28"/>
-      <c r="J33" s="28"/>
-      <c r="K33" s="28"/>
-      <c r="L33" s="28"/>
-      <c r="M33" s="28"/>
-      <c r="N33" s="28"/>
-      <c r="O33" s="28"/>
-      <c r="P33" s="28"/>
-      <c r="Q33" s="28"/>
-      <c r="R33" s="28"/>
-      <c r="S33" s="28"/>
-      <c r="T33" s="28"/>
-      <c r="U33" s="28"/>
-      <c r="V33" s="28"/>
-      <c r="W33" s="28"/>
-      <c r="X33" s="28"/>
-      <c r="Y33" s="28"/>
-      <c r="Z33" s="28"/>
-      <c r="AA33" s="28"/>
-      <c r="AB33" s="28"/>
-      <c r="AC33" s="28"/>
-      <c r="AD33" s="28"/>
-      <c r="AE33" s="28"/>
-      <c r="AF33" s="28"/>
-      <c r="AG33" s="28"/>
-      <c r="AH33" s="28"/>
-      <c r="AI33" s="28"/>
-      <c r="AJ33" s="28"/>
-      <c r="AK33" s="28"/>
-      <c r="AL33" s="28"/>
-      <c r="AM33" s="28"/>
-      <c r="AN33" s="28"/>
-      <c r="AO33" s="28"/>
-      <c r="AP33" s="28"/>
-      <c r="AQ33" s="28"/>
-      <c r="AR33" s="28"/>
-      <c r="AS33" s="28"/>
-      <c r="AT33" s="28"/>
-      <c r="AU33" s="28"/>
-      <c r="AV33" s="28"/>
-      <c r="AW33" s="28"/>
-      <c r="AX33" s="28"/>
-      <c r="AY33" s="28"/>
-      <c r="AZ33" s="28"/>
-      <c r="BA33" s="28"/>
-      <c r="BB33" s="28"/>
-      <c r="BC33" s="28"/>
-      <c r="BD33" s="28"/>
-      <c r="BE33" s="28"/>
-      <c r="BF33" s="28"/>
-      <c r="BG33" s="28"/>
-      <c r="BH33" s="28"/>
-      <c r="BI33" s="28"/>
-      <c r="BJ33" s="28"/>
-      <c r="BK33" s="28"/>
+      <c r="B36" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="C36" s="19"/>
+      <c r="D36" s="19"/>
+      <c r="E36" s="32"/>
+      <c r="F36" s="19"/>
+      <c r="G36" s="30"/>
+      <c r="H36" s="28"/>
+      <c r="I36" s="28"/>
+      <c r="J36" s="28"/>
+      <c r="K36" s="28"/>
+      <c r="L36" s="28"/>
+      <c r="M36" s="28"/>
+      <c r="N36" s="28"/>
+      <c r="O36" s="28"/>
+      <c r="P36" s="28"/>
+      <c r="Q36" s="28"/>
+      <c r="R36" s="28"/>
+      <c r="S36" s="28"/>
+      <c r="T36" s="28"/>
+      <c r="U36" s="28"/>
+      <c r="V36" s="28"/>
+      <c r="W36" s="28"/>
+      <c r="X36" s="28"/>
+      <c r="Y36" s="28"/>
+      <c r="Z36" s="28"/>
+      <c r="AA36" s="28"/>
+      <c r="AB36" s="28"/>
+      <c r="AC36" s="28"/>
+      <c r="AD36" s="28"/>
+      <c r="AE36" s="28"/>
+      <c r="AF36" s="28"/>
+      <c r="AG36" s="28"/>
+      <c r="AH36" s="28"/>
+      <c r="AI36" s="28"/>
+      <c r="AJ36" s="28"/>
+      <c r="AK36" s="28"/>
+      <c r="AL36" s="28"/>
+      <c r="AM36" s="28"/>
+      <c r="AN36" s="28"/>
+      <c r="AO36" s="28"/>
+      <c r="AP36" s="28"/>
+      <c r="AQ36" s="28"/>
+      <c r="AR36" s="28"/>
+      <c r="AS36" s="28"/>
+      <c r="AT36" s="28"/>
+      <c r="AU36" s="28"/>
+      <c r="AV36" s="28"/>
+      <c r="AW36" s="28"/>
+      <c r="AX36" s="28"/>
+      <c r="AY36" s="28"/>
+      <c r="AZ36" s="28"/>
+      <c r="BA36" s="28"/>
+      <c r="BB36" s="28"/>
+      <c r="BC36" s="28"/>
+      <c r="BD36" s="28"/>
+      <c r="BE36" s="28"/>
+      <c r="BF36" s="28"/>
+      <c r="BG36" s="28"/>
+      <c r="BH36" s="28"/>
+      <c r="BI36" s="28"/>
+      <c r="BJ36" s="28"/>
+      <c r="BK36" s="28"/>
     </row>
-    <row r="34" spans="1:63" ht="30" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="C34" s="5"/>
-      <c r="F34" s="14"/>
-      <c r="G34" s="4"/>
+    <row r="37" spans="1:63" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="C37" s="5"/>
+      <c r="F37" s="14"/>
+      <c r="G37" s="4"/>
     </row>
-    <row r="35" spans="1:63" ht="30" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="C35" s="6"/>
+    <row r="38" spans="1:63" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="C38" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -8315,8 +9370,8 @@
     <mergeCell ref="E2:F2"/>
     <mergeCell ref="C4:D4"/>
   </mergeCells>
-  <conditionalFormatting sqref="D20:D32 D6:D8">
-    <cfRule type="dataBar" priority="35">
+  <conditionalFormatting sqref="D6:D8 D20:D29 D31 D35">
+    <cfRule type="dataBar" priority="51">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -8329,23 +9384,23 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H8:BK12 H20:BK32">
-    <cfRule type="expression" dxfId="10" priority="103">
+  <conditionalFormatting sqref="H8:BK12 H20:BK29 H31:BK31 H35:BK35">
+    <cfRule type="expression" dxfId="18" priority="119">
       <formula>H$5&lt;=Heute</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H7:BK12 H20:BK32">
-    <cfRule type="expression" dxfId="9" priority="36" stopIfTrue="1">
+  <conditionalFormatting sqref="H7:BK12 H20:BK29 H31:BK31 H35:BK35">
+    <cfRule type="expression" dxfId="17" priority="52" stopIfTrue="1">
       <formula>AND(H$5&gt;=$E7+1,H$5&lt;=$E7+$F7-2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H5:BK6">
-    <cfRule type="expression" dxfId="8" priority="26">
+    <cfRule type="expression" dxfId="16" priority="42">
       <formula>H$5&lt;=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D12">
-    <cfRule type="dataBar" priority="24">
+    <cfRule type="dataBar" priority="40">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -8359,7 +9414,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D9:D11">
-    <cfRule type="dataBar" priority="21">
+    <cfRule type="dataBar" priority="37">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -8373,17 +9428,17 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H13:BK14">
-    <cfRule type="expression" dxfId="7" priority="15">
+    <cfRule type="expression" dxfId="15" priority="31">
       <formula>H$5&lt;=Heute</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H13:BK14">
-    <cfRule type="expression" dxfId="6" priority="14" stopIfTrue="1">
+    <cfRule type="expression" dxfId="14" priority="30" stopIfTrue="1">
       <formula>AND(H$5&gt;=$E13+1,H$5&lt;=$E13+$F13-2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D13:D14">
-    <cfRule type="dataBar" priority="13">
+    <cfRule type="dataBar" priority="29">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -8397,17 +9452,17 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H15:BK16">
-    <cfRule type="expression" dxfId="5" priority="11">
+    <cfRule type="expression" dxfId="13" priority="27">
       <formula>H$5&lt;=Heute</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H15:BK16">
-    <cfRule type="expression" dxfId="4" priority="10" stopIfTrue="1">
+    <cfRule type="expression" dxfId="12" priority="26" stopIfTrue="1">
       <formula>AND(H$5&gt;=$E15+1,H$5&lt;=$E15+$F15-2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D15:D16">
-    <cfRule type="dataBar" priority="9">
+    <cfRule type="dataBar" priority="25">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -8421,17 +9476,17 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H17:BK18">
-    <cfRule type="expression" dxfId="3" priority="7">
+    <cfRule type="expression" dxfId="11" priority="23">
       <formula>H$5&lt;=Heute</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H17:BK18">
-    <cfRule type="expression" dxfId="2" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="10" priority="22" stopIfTrue="1">
       <formula>AND(H$5&gt;=$E17+1,H$5&lt;=$E17+$F17-2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D17:D18">
-    <cfRule type="dataBar" priority="5">
+    <cfRule type="dataBar" priority="21">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -8445,17 +9500,17 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H19:BK19">
-    <cfRule type="expression" dxfId="1" priority="3">
+    <cfRule type="expression" dxfId="9" priority="19">
       <formula>H$5&lt;=Heute</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H19:BK19">
-    <cfRule type="expression" dxfId="0" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="8" priority="18" stopIfTrue="1">
       <formula>AND(H$5&gt;=$E19+1,H$5&lt;=$E19+$F19-2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D19">
-    <cfRule type="dataBar" priority="1">
+    <cfRule type="dataBar" priority="17">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -8466,6 +9521,102 @@
           <x14:id>{578AE1A1-2BB2-4181-A648-83EDB97DF7F2}</x14:id>
         </ext>
       </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D30">
+    <cfRule type="dataBar" priority="13">
+      <dataBar>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color theme="0" tint="-0.14999847407452621"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{364E4557-F2E9-4115-AF95-D60314F0680C}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H30:BK30">
+    <cfRule type="expression" dxfId="7" priority="15">
+      <formula>H$5&lt;=Heute</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H30:BK30">
+    <cfRule type="expression" dxfId="6" priority="14" stopIfTrue="1">
+      <formula>AND(H$5&gt;=$E30+1,H$5&lt;=$E30+$F30-2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D32">
+    <cfRule type="dataBar" priority="9">
+      <dataBar>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color theme="0" tint="-0.14999847407452621"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{289CBAE5-3ABE-4B9C-8F17-01D600B7FD89}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H32:BK32">
+    <cfRule type="expression" dxfId="5" priority="11">
+      <formula>H$5&lt;=Heute</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H32:BK32">
+    <cfRule type="expression" dxfId="4" priority="10" stopIfTrue="1">
+      <formula>AND(H$5&gt;=$E32+1,H$5&lt;=$E32+$F32-2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D34">
+    <cfRule type="dataBar" priority="5">
+      <dataBar>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color theme="0" tint="-0.14999847407452621"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{50FCDCFB-4570-4A33-8878-6D3BD99695B3}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H34:BK34">
+    <cfRule type="expression" dxfId="3" priority="7">
+      <formula>H$5&lt;=Heute</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H34:BK34">
+    <cfRule type="expression" dxfId="2" priority="6" stopIfTrue="1">
+      <formula>AND(H$5&gt;=$E34+1,H$5&lt;=$E34+$F34-2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D33">
+    <cfRule type="dataBar" priority="1">
+      <dataBar>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color theme="0" tint="-0.14999847407452621"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{A783B54A-3282-4916-BAF3-51CB57839E72}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H33:BK33">
+    <cfRule type="expression" dxfId="1" priority="3">
+      <formula>H$5&lt;=Heute</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H33:BK33">
+    <cfRule type="expression" dxfId="0" priority="2" stopIfTrue="1">
+      <formula>AND(H$5&gt;=$E33+1,H$5&lt;=$E33+$F33-2)</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
@@ -8528,7 +9679,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>D20:D32 D6:D8</xm:sqref>
+          <xm:sqref>D6:D8 D20:D29 D31 D35</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{D21556E8-F672-4265-9153-D98C5D87D31C}">
@@ -8561,7 +9712,67 @@
           <xm:sqref>D9:D11</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="27" id="{6C427F2E-2EF5-46B4-BFA6-7C68148277AC}">
+          <x14:cfRule type="dataBar" id="{DEF0B805-F08E-40F2-B697-278CC6A733AA}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="num">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>D13:D14</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{7B92A92B-57F3-4CAF-A0BD-2DFCE6BE3BD2}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="num">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>D15:D16</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{AB26E037-5CE5-45BE-B6D6-175959CEDD04}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="num">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>D17:D18</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{578AE1A1-2BB2-4181-A648-83EDB97DF7F2}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="num">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>D19</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="iconSet" priority="43" id="{6C427F2E-2EF5-46B4-BFA6-7C68148277AC}">
             <x14:iconSet iconSet="3Flags" showValue="0" custom="1">
               <x14:cfvo type="percent">
                 <xm:f>0</xm:f>
@@ -8580,41 +9791,7 @@
           <xm:sqref>F4</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="145" id="{628A03C6-EE71-4B44-A6BA-69DC45906EA6}">
-            <x14:iconSet iconSet="3Stars" showValue="0" custom="1">
-              <x14:cfvo type="percent">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="num">
-                <xm:f>1</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="num">
-                <xm:f>2</xm:f>
-              </x14:cfvo>
-              <x14:cfIcon iconSet="3Signs" iconId="1"/>
-              <x14:cfIcon iconSet="3Flags" iconId="0"/>
-              <x14:cfIcon iconSet="3Signs" iconId="0"/>
-            </x14:iconSet>
-          </x14:cfRule>
-          <xm:sqref>H7:BK12 H20:BK32</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{DEF0B805-F08E-40F2-B697-278CC6A733AA}">
-            <x14:dataBar minLength="0" maxLength="100" gradient="0">
-              <x14:cfvo type="num">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="num">
-                <xm:f>1</xm:f>
-              </x14:cfvo>
-              <x14:negativeFillColor rgb="FFFF0000"/>
-              <x14:axisColor rgb="FF000000"/>
-            </x14:dataBar>
-          </x14:cfRule>
-          <xm:sqref>D13:D14</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="16" id="{8B6C92FC-EA52-4D8A-A4AC-D98D69B552BD}">
+          <x14:cfRule type="iconSet" priority="32" id="{8B6C92FC-EA52-4D8A-A4AC-D98D69B552BD}">
             <x14:iconSet iconSet="3Stars" showValue="0" custom="1">
               <x14:cfvo type="percent">
                 <xm:f>0</xm:f>
@@ -8633,22 +9810,7 @@
           <xm:sqref>H13:BK14</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{7B92A92B-57F3-4CAF-A0BD-2DFCE6BE3BD2}">
-            <x14:dataBar minLength="0" maxLength="100" gradient="0">
-              <x14:cfvo type="num">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="num">
-                <xm:f>1</xm:f>
-              </x14:cfvo>
-              <x14:negativeFillColor rgb="FFFF0000"/>
-              <x14:axisColor rgb="FF000000"/>
-            </x14:dataBar>
-          </x14:cfRule>
-          <xm:sqref>D15:D16</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="12" id="{A093EAE9-87B9-4703-A17D-AF4D068F2329}">
+          <x14:cfRule type="iconSet" priority="28" id="{A093EAE9-87B9-4703-A17D-AF4D068F2329}">
             <x14:iconSet iconSet="3Stars" showValue="0" custom="1">
               <x14:cfvo type="percent">
                 <xm:f>0</xm:f>
@@ -8667,22 +9829,7 @@
           <xm:sqref>H15:BK16</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{AB26E037-5CE5-45BE-B6D6-175959CEDD04}">
-            <x14:dataBar minLength="0" maxLength="100" gradient="0">
-              <x14:cfvo type="num">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="num">
-                <xm:f>1</xm:f>
-              </x14:cfvo>
-              <x14:negativeFillColor rgb="FFFF0000"/>
-              <x14:axisColor rgb="FF000000"/>
-            </x14:dataBar>
-          </x14:cfRule>
-          <xm:sqref>D17:D18</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="8" id="{BA1AEAA6-BA28-46B3-99CA-1DE6F39CE90F}">
+          <x14:cfRule type="iconSet" priority="24" id="{BA1AEAA6-BA28-46B3-99CA-1DE6F39CE90F}">
             <x14:iconSet iconSet="3Stars" showValue="0" custom="1">
               <x14:cfvo type="percent">
                 <xm:f>0</xm:f>
@@ -8701,22 +9848,7 @@
           <xm:sqref>H17:BK18</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{578AE1A1-2BB2-4181-A648-83EDB97DF7F2}">
-            <x14:dataBar minLength="0" maxLength="100" gradient="0">
-              <x14:cfvo type="num">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="num">
-                <xm:f>1</xm:f>
-              </x14:cfvo>
-              <x14:negativeFillColor rgb="FFFF0000"/>
-              <x14:axisColor rgb="FF000000"/>
-            </x14:dataBar>
-          </x14:cfRule>
-          <xm:sqref>D19</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="4" id="{4B4E954B-3C89-48C4-B420-83E1CF9CCE54}">
+          <x14:cfRule type="iconSet" priority="20" id="{4B4E954B-3C89-48C4-B420-83E1CF9CCE54}">
             <x14:iconSet iconSet="3Stars" showValue="0" custom="1">
               <x14:cfvo type="percent">
                 <xm:f>0</xm:f>
@@ -8733,6 +9865,161 @@
             </x14:iconSet>
           </x14:cfRule>
           <xm:sqref>H19:BK19</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="iconSet" priority="168" id="{628A03C6-EE71-4B44-A6BA-69DC45906EA6}">
+            <x14:iconSet iconSet="3Stars" showValue="0" custom="1">
+              <x14:cfvo type="percent">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>2</xm:f>
+              </x14:cfvo>
+              <x14:cfIcon iconSet="3Signs" iconId="1"/>
+              <x14:cfIcon iconSet="3Flags" iconId="0"/>
+              <x14:cfIcon iconSet="3Signs" iconId="0"/>
+            </x14:iconSet>
+          </x14:cfRule>
+          <xm:sqref>H7:BK12 H20:BK29 H31:BK31 H35:BK35</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{364E4557-F2E9-4115-AF95-D60314F0680C}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="num">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>D30</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="iconSet" priority="16" id="{7EA132FB-8396-434F-9DE4-0E6DC490FF90}">
+            <x14:iconSet iconSet="3Stars" showValue="0" custom="1">
+              <x14:cfvo type="percent">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>2</xm:f>
+              </x14:cfvo>
+              <x14:cfIcon iconSet="3Signs" iconId="1"/>
+              <x14:cfIcon iconSet="3Flags" iconId="0"/>
+              <x14:cfIcon iconSet="3Signs" iconId="0"/>
+            </x14:iconSet>
+          </x14:cfRule>
+          <xm:sqref>H30:BK30</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{289CBAE5-3ABE-4B9C-8F17-01D600B7FD89}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="num">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>D32</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="iconSet" priority="12" id="{0BA432FB-FA12-4746-A944-4C4249EF75D3}">
+            <x14:iconSet iconSet="3Stars" showValue="0" custom="1">
+              <x14:cfvo type="percent">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>2</xm:f>
+              </x14:cfvo>
+              <x14:cfIcon iconSet="3Signs" iconId="1"/>
+              <x14:cfIcon iconSet="3Flags" iconId="0"/>
+              <x14:cfIcon iconSet="3Signs" iconId="0"/>
+            </x14:iconSet>
+          </x14:cfRule>
+          <xm:sqref>H32:BK32</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{50FCDCFB-4570-4A33-8878-6D3BD99695B3}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="num">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>D34</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="iconSet" priority="8" id="{64F16461-D14B-40E4-9BC8-56345AA00FDE}">
+            <x14:iconSet iconSet="3Stars" showValue="0" custom="1">
+              <x14:cfvo type="percent">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>2</xm:f>
+              </x14:cfvo>
+              <x14:cfIcon iconSet="3Signs" iconId="1"/>
+              <x14:cfIcon iconSet="3Flags" iconId="0"/>
+              <x14:cfIcon iconSet="3Signs" iconId="0"/>
+            </x14:iconSet>
+          </x14:cfRule>
+          <xm:sqref>H34:BK34</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{A783B54A-3282-4916-BAF3-51CB57839E72}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="num">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>D33</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="iconSet" priority="4" id="{13B340CE-9503-435A-8DC4-8BF32D494495}">
+            <x14:iconSet iconSet="3Stars" showValue="0" custom="1">
+              <x14:cfvo type="percent">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>2</xm:f>
+              </x14:cfvo>
+              <x14:cfIcon iconSet="3Signs" iconId="1"/>
+              <x14:cfIcon iconSet="3Flags" iconId="0"/>
+              <x14:cfIcon iconSet="3Signs" iconId="0"/>
+            </x14:iconSet>
+          </x14:cfRule>
+          <xm:sqref>H33:BK33</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
@@ -8754,22 +10041,22 @@
   <sheetData>
     <row r="1" spans="1:1" s="9" customFormat="1" ht="50.15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A1" s="33" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="150" x14ac:dyDescent="0.45">
       <c r="A2" s="34" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="26.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A3" s="33" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:1" s="10" customFormat="1" ht="222" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A4" s="11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>